<commit_message>
[Test Needed] Dramatically increase late-game time
</commit_message>
<xml_diff>
--- a/文档/科技市政.xlsx
+++ b/文档/科技市政.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83FF13C-F73F-46C8-858F-BB25A5052E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E682FC39-32AC-4BBA-B41B-1BF96EA55AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="168">
   <si>
     <t>Lvl</t>
   </si>
@@ -536,6 +536,13 @@
   </si>
   <si>
     <t>神秘代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机需求提升</t>
+  </si>
+  <si>
+    <t>随机需求提升</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -594,7 +601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -609,6 +616,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
-      <selection activeCell="X45" sqref="X45"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AK42" sqref="AK42:AK43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -904,6 +914,9 @@
     <col min="25" max="25" width="12.6640625"/>
     <col min="29" max="29" width="12.6640625"/>
     <col min="30" max="30" width="9.88671875" customWidth="1"/>
+    <col min="31" max="31" width="14.5546875" customWidth="1"/>
+    <col min="32" max="32" width="12.44140625" customWidth="1"/>
+    <col min="33" max="33" width="12.6640625" customWidth="1"/>
     <col min="35" max="35" width="9.33203125"/>
     <col min="38" max="38" width="9.33203125"/>
     <col min="39" max="39" width="10.109375" customWidth="1"/>
@@ -972,7 +985,7 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C34" si="0">VLOOKUP(B3,$T$3:$AB$22,9,FALSE)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>161</v>
@@ -985,7 +998,7 @@
       </c>
       <c r="G3" s="3" t="str">
         <f>_xlfn.CONCAT(D3,A3,E3,C3,F3)</f>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_POTTERY" /&gt;&lt;Set Cost="20"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_POTTERY" /&gt;&lt;Set Cost="40"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H34" si="1">VLOOKUP(B3,$T$3:$U$22,2,FALSE)</f>
@@ -999,7 +1012,7 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K34" si="2">VLOOKUP(J3,$S$46:$T$75,2,FALSE)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>164</v>
@@ -1012,7 +1025,7 @@
       </c>
       <c r="O3" s="3" t="str">
         <f>_xlfn.CONCAT(L3,I3,M3,K3,N3)</f>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CODE_OF_LAWS" /&gt;&lt;Set Cost="25"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CODE_OF_LAWS" /&gt;&lt;Set Cost="30"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -1033,11 +1046,10 @@
         <v>20</v>
       </c>
       <c r="AA3">
-        <f>AB3</f>
         <v>20</v>
       </c>
       <c r="AB3" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AC3" s="1">
         <f t="shared" ref="AC3:AC22" si="3">COUNTIF(B:B,T3)</f>
@@ -1045,7 +1057,7 @@
       </c>
       <c r="AD3" s="1">
         <f>AB3*AC3</f>
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -1057,7 +1069,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>161</v>
@@ -1070,7 +1082,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" ref="G4:G67" si="4">_xlfn.CONCAT(D4,A4,E4,C4,F4)</f>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ANIMAL_HUSBANDRY" /&gt;&lt;Set Cost="20"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ANIMAL_HUSBANDRY" /&gt;&lt;Set Cost="40"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
@@ -1084,7 +1096,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>164</v>
@@ -1097,7 +1109,7 @@
       </c>
       <c r="O4" s="3" t="str">
         <f t="shared" ref="O4:O63" si="5">_xlfn.CONCAT(L4,I4,M4,K4,N4)</f>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CRAFTSMANSHIP" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CRAFTSMANSHIP" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P4">
         <v>2</v>
@@ -1136,7 +1148,7 @@
       </c>
       <c r="AB4" s="1">
         <f>AB3+AA4</f>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AC4" s="1">
         <f t="shared" si="3"/>
@@ -1144,7 +1156,7 @@
       </c>
       <c r="AD4" s="1">
         <f t="shared" ref="AD4:AD22" si="7">AB4*AC4</f>
-        <v>250</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -1156,7 +1168,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>161</v>
@@ -1169,7 +1181,7 @@
       </c>
       <c r="G5" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MINING" /&gt;&lt;Set Cost="20"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MINING" /&gt;&lt;Set Cost="40"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -1183,7 +1195,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>164</v>
@@ -1196,7 +1208,7 @@
       </c>
       <c r="O5" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FOREIGN_TRADE" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FOREIGN_TRADE" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P5">
         <v>2</v>
@@ -1235,7 +1247,7 @@
       </c>
       <c r="AB5" s="1">
         <f>AB4+AA5</f>
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="AC5" s="1">
         <f t="shared" si="3"/>
@@ -1243,7 +1255,7 @@
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="7"/>
-        <v>270</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -1255,7 +1267,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>161</v>
@@ -1268,7 +1280,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SAILING" /&gt;&lt;Set Cost="50"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SAILING" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
@@ -1282,7 +1294,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>164</v>
@@ -1295,7 +1307,7 @@
       </c>
       <c r="O6" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRADITION" /&gt;&lt;Set Cost="90"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRADITION" /&gt;&lt;Set Cost="105"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P6">
         <v>3</v>
@@ -1334,7 +1346,7 @@
       </c>
       <c r="AB6" s="1">
         <f t="shared" ref="AB6:AB22" si="12">AB5+AA6</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" si="3"/>
@@ -1342,7 +1354,7 @@
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="7"/>
-        <v>560</v>
+        <v>640</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -1354,7 +1366,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>161</v>
@@ -1367,7 +1379,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTROLOGY" /&gt;&lt;Set Cost="50"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTROLOGY" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
@@ -1381,7 +1393,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>164</v>
@@ -1394,7 +1406,7 @@
       </c>
       <c r="O7" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_STATE_WORKFORCE" /&gt;&lt;Set Cost="120"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_STATE_WORKFORCE" /&gt;&lt;Set Cost="135"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P7">
         <v>3</v>
@@ -1425,15 +1437,15 @@
         <v>105</v>
       </c>
       <c r="Z7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA7">
         <f t="shared" si="10"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" si="12"/>
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" si="3"/>
@@ -1441,7 +1453,7 @@
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="7"/>
-        <v>800</v>
+        <v>920</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1453,7 +1465,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>161</v>
@@ -1466,7 +1478,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRRIGATION" /&gt;&lt;Set Cost="50"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRRIGATION" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
@@ -1480,7 +1492,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>164</v>
@@ -1493,7 +1505,7 @@
       </c>
       <c r="O8" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EARLY_EMPIRE" /&gt;&lt;Set Cost="120"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EARLY_EMPIRE" /&gt;&lt;Set Cost="135"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P8">
         <v>3</v>
@@ -1528,11 +1540,11 @@
       </c>
       <c r="AA8">
         <f t="shared" si="10"/>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AB8" s="1">
         <f t="shared" si="12"/>
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="AC8" s="1">
         <f t="shared" si="3"/>
@@ -1540,7 +1552,7 @@
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="7"/>
-        <v>1120</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -1552,7 +1564,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>161</v>
@@ -1565,7 +1577,7 @@
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ARCHERY" /&gt;&lt;Set Cost="50"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ARCHERY" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
@@ -1579,7 +1591,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>164</v>
@@ -1592,7 +1604,7 @@
       </c>
       <c r="O9" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MYSTICISM" /&gt;&lt;Set Cost="90"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MYSTICISM" /&gt;&lt;Set Cost="105"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P9">
         <v>3</v>
@@ -1627,11 +1639,11 @@
       </c>
       <c r="AA9">
         <f t="shared" si="10"/>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AB9" s="1">
         <f t="shared" si="12"/>
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="AC9" s="1">
         <f t="shared" si="3"/>
@@ -1639,7 +1651,7 @@
       </c>
       <c r="AD9" s="1">
         <f t="shared" si="7"/>
-        <v>1520</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -1651,7 +1663,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>161</v>
@@ -1664,7 +1676,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_WRITING" /&gt;&lt;Set Cost="50"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_WRITING" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
@@ -1678,7 +1690,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>164</v>
@@ -1691,7 +1703,7 @@
       </c>
       <c r="O10" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GAMES_RECREATION" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GAMES_RECREATION" /&gt;&lt;Set Cost="190"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P10">
         <v>4</v>
@@ -1722,15 +1734,15 @@
         <v>375</v>
       </c>
       <c r="Z10">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AA10">
         <f t="shared" si="10"/>
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AB10" s="1">
         <f t="shared" si="12"/>
-        <v>500</v>
+        <v>580</v>
       </c>
       <c r="AC10" s="1">
         <f t="shared" si="3"/>
@@ -1738,7 +1750,7 @@
       </c>
       <c r="AD10" s="1">
         <f t="shared" si="7"/>
-        <v>2500</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -1750,7 +1762,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>161</v>
@@ -1763,7 +1775,7 @@
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASONRY" /&gt;&lt;Set Cost="90"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASONRY" /&gt;&lt;Set Cost="110"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
@@ -1777,7 +1789,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>164</v>
@@ -1790,7 +1802,7 @@
       </c>
       <c r="O11" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_POLITICAL_PHILOSOPHY" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_POLITICAL_PHILOSOPHY" /&gt;&lt;Set Cost="190"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P11">
         <v>4</v>
@@ -1821,15 +1833,15 @@
         <v>485</v>
       </c>
       <c r="Z11">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AA11">
         <f t="shared" si="10"/>
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="AB11" s="1">
         <f t="shared" si="12"/>
-        <v>640</v>
+        <v>770</v>
       </c>
       <c r="AC11" s="1">
         <f t="shared" si="3"/>
@@ -1837,7 +1849,7 @@
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="7"/>
-        <v>2560</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -1849,7 +1861,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>161</v>
@@ -1862,7 +1874,7 @@
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BRONZE_WORKING" /&gt;&lt;Set Cost="90"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BRONZE_WORKING" /&gt;&lt;Set Cost="110"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
@@ -1876,7 +1888,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>164</v>
@@ -1889,7 +1901,7 @@
       </c>
       <c r="O12" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DRAMA_POETRY" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DRAMA_POETRY" /&gt;&lt;Set Cost="190"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P12">
         <v>4</v>
@@ -1924,11 +1936,11 @@
       </c>
       <c r="AA12">
         <f t="shared" si="10"/>
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="AB12" s="1">
         <f t="shared" si="12"/>
-        <v>820</v>
+        <v>1000</v>
       </c>
       <c r="AC12" s="1">
         <f t="shared" si="3"/>
@@ -1936,7 +1948,7 @@
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="7"/>
-        <v>3280</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -1948,7 +1960,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>161</v>
@@ -1961,7 +1973,7 @@
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_THE_WHEEL" /&gt;&lt;Set Cost="90"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_THE_WHEEL" /&gt;&lt;Set Cost="110"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
@@ -1975,7 +1987,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>164</v>
@@ -1988,7 +2000,7 @@
       </c>
       <c r="O13" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRAINING" /&gt;&lt;Set Cost="195"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRAINING" /&gt;&lt;Set Cost="250"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P13">
         <v>5</v>
@@ -2019,15 +2031,15 @@
         <v>1150</v>
       </c>
       <c r="Z13">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="AA13">
         <f t="shared" si="10"/>
-        <v>220</v>
+        <v>310</v>
       </c>
       <c r="AB13" s="1">
         <f t="shared" si="12"/>
-        <v>1040</v>
+        <v>1310</v>
       </c>
       <c r="AC13" s="1">
         <f t="shared" si="3"/>
@@ -2035,7 +2047,7 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="7"/>
-        <v>4160</v>
+        <v>5240</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -2047,7 +2059,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>161</v>
@@ -2060,7 +2072,7 @@
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CELESTIAL_NAVIGATION" /&gt;&lt;Set Cost="140"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CELESTIAL_NAVIGATION" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
@@ -2074,7 +2086,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>164</v>
@@ -2087,7 +2099,7 @@
       </c>
       <c r="O14" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DEFENSIVE_TACTICS" /&gt;&lt;Set Cost="255"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DEFENSIVE_TACTICS" /&gt;&lt;Set Cost="310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P14">
         <v>5</v>
@@ -2118,15 +2130,15 @@
         <v>1600</v>
       </c>
       <c r="Z14">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="AA14">
         <f t="shared" si="10"/>
-        <v>260</v>
+        <v>390</v>
       </c>
       <c r="AB14" s="1">
         <f t="shared" si="12"/>
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="AC14" s="1">
         <f t="shared" si="3"/>
@@ -2134,7 +2146,7 @@
       </c>
       <c r="AD14" s="1">
         <f t="shared" si="7"/>
-        <v>5200</v>
+        <v>6800</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -2146,7 +2158,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>161</v>
@@ -2159,7 +2171,7 @@
       </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CURRENCY" /&gt;&lt;Set Cost="140"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CURRENCY" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
@@ -2173,7 +2185,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>164</v>
@@ -2186,7 +2198,7 @@
       </c>
       <c r="O15" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RECORDED_HISTORY" /&gt;&lt;Set Cost="255"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RECORDED_HISTORY" /&gt;&lt;Set Cost="310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P15">
         <v>5</v>
@@ -2217,15 +2229,15 @@
         <v>2350</v>
       </c>
       <c r="Z15">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="AA15">
         <f t="shared" si="10"/>
-        <v>300</v>
+        <v>470</v>
       </c>
       <c r="AB15" s="1">
         <f t="shared" si="12"/>
-        <v>1600</v>
+        <v>2170</v>
       </c>
       <c r="AC15" s="1">
         <f t="shared" si="3"/>
@@ -2233,7 +2245,7 @@
       </c>
       <c r="AD15" s="1">
         <f t="shared" si="7"/>
-        <v>6400</v>
+        <v>8680</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2245,7 +2257,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>161</v>
@@ -2258,7 +2270,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_HORSEBACK_RIDING" /&gt;&lt;Set Cost="140"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_HORSEBACK_RIDING" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
@@ -2272,7 +2284,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>164</v>
@@ -2285,7 +2297,7 @@
       </c>
       <c r="O16" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THEOLOGY" /&gt;&lt;Set Cost="195"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THEOLOGY" /&gt;&lt;Set Cost="250"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P16">
         <v>5</v>
@@ -2316,15 +2328,15 @@
         <v>3100</v>
       </c>
       <c r="Z16">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="AA16">
         <f t="shared" si="10"/>
-        <v>360</v>
+        <v>570</v>
       </c>
       <c r="AB16" s="1">
         <f t="shared" si="12"/>
-        <v>1960</v>
+        <v>2740</v>
       </c>
       <c r="AC16" s="1">
         <f t="shared" si="3"/>
@@ -2332,7 +2344,7 @@
       </c>
       <c r="AD16" s="1">
         <f t="shared" si="7"/>
-        <v>9800</v>
+        <v>13700</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
@@ -2344,7 +2356,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>161</v>
@@ -2357,7 +2369,7 @@
       </c>
       <c r="G17" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRON_WORKING" /&gt;&lt;Set Cost="140"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRON_WORKING" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
@@ -2371,7 +2383,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>164</v>
@@ -2384,7 +2396,7 @@
       </c>
       <c r="O17" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NAVAL_TRADITION" /&gt;&lt;Set Cost="275"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NAVAL_TRADITION" /&gt;&lt;Set Cost="355"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P17">
         <v>6</v>
@@ -2415,15 +2427,15 @@
         <v>4100</v>
       </c>
       <c r="Z17">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="AA17">
         <f t="shared" si="10"/>
-        <v>420</v>
+        <v>670</v>
       </c>
       <c r="AB17" s="1">
         <f t="shared" si="12"/>
-        <v>2380</v>
+        <v>3410</v>
       </c>
       <c r="AC17" s="1">
         <f t="shared" si="3"/>
@@ -2431,7 +2443,7 @@
       </c>
       <c r="AD17" s="1">
         <f t="shared" si="7"/>
-        <v>7140</v>
+        <v>10230</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
@@ -2443,7 +2455,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>161</v>
@@ -2456,7 +2468,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SHIPBUILDING" /&gt;&lt;Set Cost="200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SHIPBUILDING" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
@@ -2470,7 +2482,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
-        <v>365</v>
+        <v>445</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>164</v>
@@ -2483,7 +2495,7 @@
       </c>
       <c r="O18" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FEUDALISM" /&gt;&lt;Set Cost="365"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FEUDALISM" /&gt;&lt;Set Cost="445"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P18">
         <v>6</v>
@@ -2514,15 +2526,15 @@
         <v>5100</v>
       </c>
       <c r="Z18">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="AA18">
         <f t="shared" si="10"/>
-        <v>480</v>
+        <v>790</v>
       </c>
       <c r="AB18" s="1">
         <f t="shared" si="12"/>
-        <v>2860</v>
+        <v>4200</v>
       </c>
       <c r="AC18" s="1">
         <f t="shared" si="3"/>
@@ -2530,7 +2542,7 @@
       </c>
       <c r="AD18" s="1">
         <f t="shared" si="7"/>
-        <v>17160</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
@@ -2542,7 +2554,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>161</v>
@@ -2555,7 +2567,7 @@
       </c>
       <c r="G19" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MATHEMATICS" /&gt;&lt;Set Cost="200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MATHEMATICS" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
@@ -2569,7 +2581,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
-        <v>365</v>
+        <v>445</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>164</v>
@@ -2582,7 +2594,7 @@
       </c>
       <c r="O19" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_SERVICE" /&gt;&lt;Set Cost="365"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_SERVICE" /&gt;&lt;Set Cost="445"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P19">
         <v>6</v>
@@ -2613,15 +2625,15 @@
         <v>6400</v>
       </c>
       <c r="Z19">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="AA19">
         <f t="shared" si="10"/>
-        <v>540</v>
+        <v>910</v>
       </c>
       <c r="AB19" s="1">
         <f t="shared" si="12"/>
-        <v>3400</v>
+        <v>5110</v>
       </c>
       <c r="AC19" s="1">
         <f t="shared" si="3"/>
@@ -2629,7 +2641,10 @@
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="7"/>
-        <v>10200</v>
+        <v>15330</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
@@ -2641,7 +2656,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>161</v>
@@ -2654,7 +2669,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CONSTRUCTION" /&gt;&lt;Set Cost="200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CONSTRUCTION" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
@@ -2668,7 +2683,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>505</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>164</v>
@@ -2681,7 +2696,7 @@
       </c>
       <c r="O20" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCENARIES" /&gt;&lt;Set Cost="400"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCENARIES" /&gt;&lt;Set Cost="505"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P20">
         <v>7</v>
@@ -2712,15 +2727,15 @@
         <v>7700</v>
       </c>
       <c r="Z20">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="AA20">
         <f t="shared" si="10"/>
-        <v>620</v>
+        <v>1050</v>
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="12"/>
-        <v>4020</v>
+        <v>6160</v>
       </c>
       <c r="AC20" s="1">
         <f t="shared" si="3"/>
@@ -2728,7 +2743,11 @@
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="7"/>
-        <v>24120</v>
+        <v>36960</v>
+      </c>
+      <c r="AE20">
+        <f>AB20+0.5*AA21</f>
+        <v>6755</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
@@ -2740,7 +2759,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>161</v>
@@ -2753,7 +2772,7 @@
       </c>
       <c r="G21" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ENGINEERING" /&gt;&lt;Set Cost="200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ENGINEERING" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
@@ -2767,7 +2786,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="2"/>
-        <v>490</v>
+        <v>595</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>164</v>
@@ -2780,7 +2799,7 @@
       </c>
       <c r="O21" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MEDIEVAL_FAIRES" /&gt;&lt;Set Cost="490"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MEDIEVAL_FAIRES" /&gt;&lt;Set Cost="595"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P21">
         <v>7</v>
@@ -2811,15 +2830,15 @@
         <v>8800</v>
       </c>
       <c r="Z21">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="AA21">
         <f t="shared" si="10"/>
-        <v>700</v>
+        <v>1190</v>
       </c>
       <c r="AB21" s="1">
         <f t="shared" si="12"/>
-        <v>4720</v>
+        <v>7350</v>
       </c>
       <c r="AC21" s="1">
         <f t="shared" si="3"/>
@@ -2827,7 +2846,7 @@
       </c>
       <c r="AD21" s="1">
         <f t="shared" si="7"/>
-        <v>4720</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
@@ -2839,7 +2858,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>161</v>
@@ -2852,7 +2871,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_TACTICS" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_TACTICS" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
@@ -2866,7 +2885,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
-        <v>490</v>
+        <v>595</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>164</v>
@@ -2879,7 +2898,7 @@
       </c>
       <c r="O22" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GUILDS" /&gt;&lt;Set Cost="490"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GUILDS" /&gt;&lt;Set Cost="595"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P22">
         <v>7</v>
@@ -2910,15 +2929,15 @@
         <v>9500</v>
       </c>
       <c r="Z22">
-        <v>80</v>
+        <v>-540</v>
       </c>
       <c r="AA22">
         <f t="shared" si="10"/>
-        <v>780</v>
+        <v>650</v>
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="12"/>
-        <v>5500</v>
+        <v>8000</v>
       </c>
       <c r="AC22" s="1">
         <f t="shared" si="3"/>
@@ -2926,7 +2945,7 @@
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="7"/>
-        <v>5500</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
@@ -2938,7 +2957,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>161</v>
@@ -2951,7 +2970,7 @@
       </c>
       <c r="G23" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_APPRENTICESHIP" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_APPRENTICESHIP" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
@@ -2965,7 +2984,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="2"/>
-        <v>400</v>
+        <v>505</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>164</v>
@@ -2978,7 +2997,7 @@
       </c>
       <c r="O23" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIVINE_RIGHT" /&gt;&lt;Set Cost="400"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIVINE_RIGHT" /&gt;&lt;Set Cost="505"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P23">
         <v>7</v>
@@ -2999,7 +3018,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>161</v>
@@ -3012,7 +3031,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MACHINERY" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MACHINERY" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
@@ -3026,7 +3045,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
-        <v>540</v>
+        <v>690</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>164</v>
@@ -3039,7 +3058,7 @@
       </c>
       <c r="O24" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXPLORATION" /&gt;&lt;Set Cost="540"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXPLORATION" /&gt;&lt;Set Cost="690"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P24">
         <v>8</v>
@@ -3111,7 +3130,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>161</v>
@@ -3124,7 +3143,7 @@
       </c>
       <c r="G25" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_EDUCATION" /&gt;&lt;Set Cost="380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_EDUCATION" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
@@ -3138,7 +3157,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
-        <v>660</v>
+        <v>810</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>164</v>
@@ -3151,7 +3170,7 @@
       </c>
       <c r="O25" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_HUMANISM" /&gt;&lt;Set Cost="660"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_HUMANISM" /&gt;&lt;Set Cost="810"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P25">
         <v>8</v>
@@ -3181,50 +3200,50 @@
         <v>0</v>
       </c>
       <c r="Y25">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Z25">
         <f>0+Y25</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AA25">
         <v>0</v>
       </c>
       <c r="AB25">
         <f t="shared" ref="AB25:AB28" si="14">Z25-0.5*AA25</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AC25">
         <f t="shared" ref="AC25:AC28" si="15">Z25+0.5*AA25</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AD25">
         <f t="shared" ref="AD25:AD44" si="16">Z25*W25</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AE25">
         <f t="shared" ref="AE25:AE44" si="17">AD3</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="AF25" s="4">
         <f>AD25+AD26+AD27</f>
-        <v>565</v>
+        <v>650</v>
       </c>
       <c r="AG25" s="4">
         <f>AE25+AE26+AE27</f>
-        <v>580</v>
+        <v>800</v>
       </c>
       <c r="AH25" s="4">
         <f>AF25</f>
-        <v>565</v>
+        <v>650</v>
       </c>
       <c r="AI25" s="4">
         <f>AG25</f>
-        <v>580</v>
+        <v>800</v>
       </c>
       <c r="AJ25" s="4">
         <f>AH25-AI25</f>
-        <v>-15</v>
+        <v>-150</v>
       </c>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
@@ -3239,7 +3258,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>161</v>
@@ -3252,7 +3271,7 @@
       </c>
       <c r="G26" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STIRRUPS" /&gt;&lt;Set Cost="380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STIRRUPS" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
@@ -3266,7 +3285,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="2"/>
-        <v>660</v>
+        <v>810</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>164</v>
@@ -3279,7 +3298,7 @@
       </c>
       <c r="O26" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIPLOMATIC_SERVICE" /&gt;&lt;Set Cost="660"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIPLOMATIC_SERVICE" /&gt;&lt;Set Cost="810"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P26">
         <v>8</v>
@@ -3310,30 +3329,30 @@
       </c>
       <c r="Y26">
         <f>Y25+X26</f>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="Z26">
         <f>Z25+Y26</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AA26">
         <v>0</v>
       </c>
       <c r="AB26">
         <f t="shared" si="14"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AC26">
         <f t="shared" si="15"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AD26">
         <f t="shared" si="16"/>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="AE26">
         <f t="shared" si="17"/>
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
@@ -3353,7 +3372,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>161</v>
@@ -3366,7 +3385,7 @@
       </c>
       <c r="G27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_ENGINEERING" /&gt;&lt;Set Cost="380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_ENGINEERING" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
@@ -3380,7 +3399,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="2"/>
-        <v>540</v>
+        <v>690</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>164</v>
@@ -3393,7 +3412,7 @@
       </c>
       <c r="O27" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_REFORMED_CHURCH" /&gt;&lt;Set Cost="540"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_REFORMED_CHURCH" /&gt;&lt;Set Cost="690"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P27">
         <v>8</v>
@@ -3424,30 +3443,30 @@
       </c>
       <c r="Y27">
         <f t="shared" ref="Y27:Y43" si="19">Y26+X27</f>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="Z27">
         <f t="shared" ref="Z27:Z43" si="20">Z26+Y27</f>
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="AA27">
         <v>30</v>
       </c>
       <c r="AB27">
         <f t="shared" si="14"/>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="AC27">
         <f t="shared" si="15"/>
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="AD27">
         <f t="shared" si="16"/>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="AE27">
         <f t="shared" si="17"/>
-        <v>270</v>
+        <v>330</v>
       </c>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
@@ -3467,7 +3486,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>161</v>
@@ -3480,7 +3499,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CASTLES" /&gt;&lt;Set Cost="380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CASTLES" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
@@ -3494,7 +3513,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="2"/>
-        <v>785</v>
+        <v>1000</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>164</v>
@@ -3507,7 +3526,7 @@
       </c>
       <c r="O28" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCANTILISM" /&gt;&lt;Set Cost="785"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCANTILISM" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P28">
         <v>9</v>
@@ -3534,54 +3553,54 @@
         <v>3</v>
       </c>
       <c r="X28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Y28">
         <f t="shared" si="19"/>
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="Z28">
         <f t="shared" si="20"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="AA28">
         <v>0</v>
       </c>
       <c r="AB28">
         <f t="shared" si="14"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="AC28">
         <f t="shared" si="15"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="AD28">
         <f t="shared" si="16"/>
-        <v>480</v>
+        <v>570</v>
       </c>
       <c r="AE28">
         <f t="shared" si="17"/>
-        <v>560</v>
+        <v>640</v>
       </c>
       <c r="AF28" s="4">
         <f>AD28+AD29</f>
-        <v>1155</v>
+        <v>1410</v>
       </c>
       <c r="AG28" s="4">
         <f>AE28+AE29</f>
-        <v>1360</v>
+        <v>1560</v>
       </c>
       <c r="AH28" s="4">
         <f>AH25+AF28</f>
-        <v>1720</v>
+        <v>2060</v>
       </c>
       <c r="AI28" s="4">
         <f>AI25+AG28</f>
-        <v>1940</v>
+        <v>2360</v>
       </c>
       <c r="AJ28" s="4">
         <f>AH28-AI28</f>
-        <v>-220</v>
+        <v>-300</v>
       </c>
       <c r="AK28" s="4"/>
       <c r="AL28" s="4"/>
@@ -3596,7 +3615,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>580</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>161</v>
@@ -3609,7 +3628,7 @@
       </c>
       <c r="G29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CARTOGRAPHY" /&gt;&lt;Set Cost="500"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CARTOGRAPHY" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
@@ -3623,7 +3642,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
-        <v>785</v>
+        <v>1000</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>164</v>
@@ -3636,7 +3655,7 @@
       </c>
       <c r="O29" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THE_ENLIGHTENMENT" /&gt;&lt;Set Cost="785"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THE_ENLIGHTENMENT" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P29">
         <v>9</v>
@@ -3662,34 +3681,34 @@
         <v>3</v>
       </c>
       <c r="X29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Y29">
         <f t="shared" si="19"/>
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="Z29">
         <f t="shared" si="20"/>
-        <v>225</v>
+        <v>280</v>
       </c>
       <c r="AA29">
         <v>60</v>
       </c>
       <c r="AB29">
         <f t="shared" ref="AB29" si="21">Z29-0.5*AA29</f>
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="AC29">
         <f t="shared" ref="AC29" si="22">Z29+0.5*AA29</f>
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="AD29">
         <f t="shared" si="16"/>
-        <v>675</v>
+        <v>840</v>
       </c>
       <c r="AE29">
         <f t="shared" si="17"/>
-        <v>800</v>
+        <v>920</v>
       </c>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
@@ -3709,7 +3728,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>580</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>161</v>
@@ -3722,7 +3741,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASS_PRODUCTION" /&gt;&lt;Set Cost="500"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASS_PRODUCTION" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
@@ -3736,7 +3755,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
-        <v>945</v>
+        <v>1245</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>164</v>
@@ -3749,7 +3768,7 @@
       </c>
       <c r="O30" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLONIALISM" /&gt;&lt;Set Cost="945"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLONIALISM" /&gt;&lt;Set Cost="1245"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P30">
         <v>10</v>
@@ -3779,50 +3798,50 @@
       </c>
       <c r="Y30">
         <f t="shared" si="19"/>
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="Z30">
         <f t="shared" si="20"/>
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="AA30">
         <v>90</v>
       </c>
       <c r="AB30">
         <f t="shared" ref="AB30:AB44" si="23">Z30-0.5*AA30</f>
-        <v>275</v>
+        <v>355</v>
       </c>
       <c r="AC30">
         <f t="shared" ref="AC30:AC44" si="24">Z30+0.5*AA30</f>
-        <v>365</v>
+        <v>445</v>
       </c>
       <c r="AD30">
         <f t="shared" si="16"/>
-        <v>960</v>
+        <v>1200</v>
       </c>
       <c r="AE30">
         <f t="shared" si="17"/>
-        <v>1120</v>
+        <v>1280</v>
       </c>
       <c r="AF30" s="4">
         <f>AD30+AD31</f>
-        <v>2295</v>
+        <v>2850</v>
       </c>
       <c r="AG30" s="4">
         <f>AE30+AE31</f>
-        <v>2640</v>
+        <v>3000</v>
       </c>
       <c r="AH30" s="4">
         <f>AH28+AF30</f>
-        <v>4015</v>
+        <v>4910</v>
       </c>
       <c r="AI30" s="4">
         <f>AI28+AG30</f>
-        <v>4580</v>
+        <v>5360</v>
       </c>
       <c r="AJ30" s="4">
         <f>AH30-AI30</f>
-        <v>-565</v>
+        <v>-450</v>
       </c>
       <c r="AK30" s="4"/>
       <c r="AL30" s="4"/>
@@ -3837,7 +3856,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>580</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>161</v>
@@ -3850,7 +3869,7 @@
       </c>
       <c r="G31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BANKING" /&gt;&lt;Set Cost="500"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BANKING" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
@@ -3864,7 +3883,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="2"/>
-        <v>1095</v>
+        <v>1395</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>164</v>
@@ -3877,7 +3896,7 @@
       </c>
       <c r="O31" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_ENGINEERING" /&gt;&lt;Set Cost="1095"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_ENGINEERING" /&gt;&lt;Set Cost="1395"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P31">
         <v>10</v>
@@ -3907,30 +3926,30 @@
       </c>
       <c r="Y31">
         <f t="shared" si="19"/>
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="Z31">
         <f t="shared" si="20"/>
-        <v>445</v>
+        <v>550</v>
       </c>
       <c r="AA31">
         <v>90</v>
       </c>
       <c r="AB31">
         <f t="shared" si="23"/>
-        <v>400</v>
+        <v>505</v>
       </c>
       <c r="AC31">
         <f t="shared" si="24"/>
-        <v>490</v>
+        <v>595</v>
       </c>
       <c r="AD31">
         <f t="shared" si="16"/>
-        <v>1335</v>
+        <v>1650</v>
       </c>
       <c r="AE31">
         <f t="shared" si="17"/>
-        <v>1520</v>
+        <v>1720</v>
       </c>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
@@ -3950,7 +3969,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>580</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>161</v>
@@ -3963,7 +3982,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUNPOWDER" /&gt;&lt;Set Cost="500"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUNPOWDER" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
@@ -3977,7 +3996,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="2"/>
-        <v>1095</v>
+        <v>1395</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>164</v>
@@ -3990,7 +4009,7 @@
       </c>
       <c r="O32" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATIONALISM" /&gt;&lt;Set Cost="1095"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATIONALISM" /&gt;&lt;Set Cost="1395"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P32">
         <v>10</v>
@@ -4016,54 +4035,54 @@
         <v>3</v>
       </c>
       <c r="X32">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Y32">
         <f t="shared" si="19"/>
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="Z32">
         <f t="shared" si="20"/>
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="AA32">
         <v>120</v>
       </c>
       <c r="AB32">
         <f t="shared" si="23"/>
-        <v>540</v>
+        <v>690</v>
       </c>
       <c r="AC32">
         <f t="shared" si="24"/>
-        <v>660</v>
+        <v>810</v>
       </c>
       <c r="AD32">
         <f t="shared" si="16"/>
-        <v>1800</v>
+        <v>2250</v>
       </c>
       <c r="AE32">
         <f t="shared" si="17"/>
-        <v>2500</v>
+        <v>2900</v>
       </c>
       <c r="AF32" s="4">
         <f>AD32+AD33</f>
-        <v>3370</v>
+        <v>4250</v>
       </c>
       <c r="AG32" s="4">
         <f>AE32+AE33</f>
-        <v>5060</v>
+        <v>5980</v>
       </c>
       <c r="AH32" s="4">
         <f>AH30+AF32</f>
-        <v>7385</v>
+        <v>9160</v>
       </c>
       <c r="AI32" s="4">
         <f>AI30+AG32</f>
-        <v>9640</v>
+        <v>11340</v>
       </c>
       <c r="AJ32" s="4">
         <f>AH32-AI32</f>
-        <v>-2255</v>
+        <v>-2180</v>
       </c>
       <c r="AK32" s="4"/>
       <c r="AL32" s="4"/>
@@ -4078,7 +4097,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>580</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>161</v>
@@ -4091,7 +4110,7 @@
       </c>
       <c r="G33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PRINTING" /&gt;&lt;Set Cost="500"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PRINTING" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
@@ -4105,7 +4124,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="2"/>
-        <v>945</v>
+        <v>1245</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>164</v>
@@ -4118,7 +4137,7 @@
       </c>
       <c r="O33" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_OPERA_BALLET" /&gt;&lt;Set Cost="945"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_OPERA_BALLET" /&gt;&lt;Set Cost="1245"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P33">
         <v>10</v>
@@ -4145,34 +4164,34 @@
         <v>2</v>
       </c>
       <c r="X33">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Y33">
         <f t="shared" si="19"/>
-        <v>185</v>
+        <v>250</v>
       </c>
       <c r="Z33">
         <f t="shared" si="20"/>
-        <v>785</v>
+        <v>1000</v>
       </c>
       <c r="AA33">
         <v>0</v>
       </c>
       <c r="AB33">
         <f t="shared" si="23"/>
-        <v>785</v>
+        <v>1000</v>
       </c>
       <c r="AC33">
         <f t="shared" si="24"/>
-        <v>785</v>
+        <v>1000</v>
       </c>
       <c r="AD33">
         <f t="shared" si="16"/>
-        <v>1570</v>
+        <v>2000</v>
       </c>
       <c r="AE33">
         <f t="shared" si="17"/>
-        <v>2560</v>
+        <v>3080</v>
       </c>
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
@@ -4192,7 +4211,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>770</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>161</v>
@@ -4205,7 +4224,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SQUARE_RIGGING" /&gt;&lt;Set Cost="640"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SQUARE_RIGGING" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
@@ -4219,7 +4238,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="2"/>
-        <v>1230</v>
+        <v>1635</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>164</v>
@@ -4232,7 +4251,7 @@
       </c>
       <c r="O34" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATURAL_HISTORY" /&gt;&lt;Set Cost="1230"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATURAL_HISTORY" /&gt;&lt;Set Cost="1635"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P34">
         <v>11</v>
@@ -4259,54 +4278,54 @@
         <v>4</v>
       </c>
       <c r="X34">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="Y34">
         <f t="shared" si="19"/>
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="Z34">
         <f t="shared" si="20"/>
-        <v>1020</v>
+        <v>1320</v>
       </c>
       <c r="AA34">
         <v>150</v>
       </c>
       <c r="AB34">
         <f t="shared" si="23"/>
-        <v>945</v>
+        <v>1245</v>
       </c>
       <c r="AC34">
         <f t="shared" si="24"/>
-        <v>1095</v>
+        <v>1395</v>
       </c>
       <c r="AD34">
         <f t="shared" si="16"/>
-        <v>4080</v>
+        <v>5280</v>
       </c>
       <c r="AE34">
         <f t="shared" si="17"/>
-        <v>3280</v>
+        <v>4000</v>
       </c>
       <c r="AF34" s="4">
         <f>AD34+AD35</f>
-        <v>7995</v>
+        <v>10410</v>
       </c>
       <c r="AG34" s="4">
         <f>AE34+AE35</f>
-        <v>7440</v>
+        <v>9240</v>
       </c>
       <c r="AH34" s="4">
         <f>AH32+AF34</f>
-        <v>15380</v>
+        <v>19570</v>
       </c>
       <c r="AI34" s="4">
         <f>AI32+AG34</f>
-        <v>17080</v>
+        <v>20580</v>
       </c>
       <c r="AJ34" s="4">
         <f>AH34-AI34</f>
-        <v>-1700</v>
+        <v>-1010</v>
       </c>
       <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
@@ -4321,7 +4340,7 @@
       </c>
       <c r="C35">
         <f t="shared" ref="C35:C66" si="25">VLOOKUP(B35,$T$3:$AB$22,9,FALSE)</f>
-        <v>640</v>
+        <v>770</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>161</v>
@@ -4334,7 +4353,7 @@
       </c>
       <c r="G35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTRONOMY" /&gt;&lt;Set Cost="640"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTRONOMY" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H35">
         <f t="shared" ref="H35:H66" si="26">VLOOKUP(B35,$T$3:$U$22,2,FALSE)</f>
@@ -4348,7 +4367,7 @@
       </c>
       <c r="K35">
         <f t="shared" ref="K35:K63" si="27">VLOOKUP(J35,$S$46:$T$75,2,FALSE)</f>
-        <v>1380</v>
+        <v>1785</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>164</v>
@@ -4361,7 +4380,7 @@
       </c>
       <c r="O35" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SCORCHED_EARTH" /&gt;&lt;Set Cost="1380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SCORCHED_EARTH" /&gt;&lt;Set Cost="1785"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P35">
         <v>11</v>
@@ -4387,34 +4406,34 @@
         <v>3</v>
       </c>
       <c r="X35">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="Y35">
         <f t="shared" si="19"/>
-        <v>285</v>
+        <v>390</v>
       </c>
       <c r="Z35">
         <f t="shared" si="20"/>
-        <v>1305</v>
+        <v>1710</v>
       </c>
       <c r="AA35">
         <v>150</v>
       </c>
       <c r="AB35">
         <f t="shared" si="23"/>
-        <v>1230</v>
+        <v>1635</v>
       </c>
       <c r="AC35">
         <f t="shared" si="24"/>
-        <v>1380</v>
+        <v>1785</v>
       </c>
       <c r="AD35">
         <f t="shared" si="16"/>
-        <v>3915</v>
+        <v>5130</v>
       </c>
       <c r="AE35">
         <f t="shared" si="17"/>
-        <v>4160</v>
+        <v>5240</v>
       </c>
       <c r="AF35" s="4"/>
       <c r="AG35" s="4"/>
@@ -4434,7 +4453,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="25"/>
-        <v>640</v>
+        <v>770</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>161</v>
@@ -4447,7 +4466,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_METAL_CASTING" /&gt;&lt;Set Cost="640"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_METAL_CASTING" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H36">
         <f t="shared" si="26"/>
@@ -4461,7 +4480,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="27"/>
-        <v>1380</v>
+        <v>1785</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>164</v>
@@ -4474,7 +4493,7 @@
       </c>
       <c r="O36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_URBANIZATION" /&gt;&lt;Set Cost="1380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_URBANIZATION" /&gt;&lt;Set Cost="1785"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P36">
         <v>11</v>
@@ -4500,54 +4519,54 @@
         <v>4</v>
       </c>
       <c r="X36">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="Y36">
         <f t="shared" si="19"/>
-        <v>335</v>
+        <v>480</v>
       </c>
       <c r="Z36">
         <f t="shared" si="20"/>
-        <v>1640</v>
+        <v>2190</v>
       </c>
       <c r="AA36">
         <v>120</v>
       </c>
       <c r="AB36">
         <f t="shared" si="23"/>
-        <v>1580</v>
+        <v>2130</v>
       </c>
       <c r="AC36">
         <f t="shared" si="24"/>
-        <v>1700</v>
+        <v>2250</v>
       </c>
       <c r="AD36">
         <f t="shared" si="16"/>
-        <v>6560</v>
+        <v>8760</v>
       </c>
       <c r="AE36">
         <f t="shared" si="17"/>
-        <v>5200</v>
+        <v>6800</v>
       </c>
       <c r="AF36" s="4">
         <f>AD36+AD37</f>
-        <v>10610</v>
+        <v>14280</v>
       </c>
       <c r="AG36" s="4">
         <f>AE36+AE37</f>
-        <v>11600</v>
+        <v>15480</v>
       </c>
       <c r="AH36" s="4">
         <f t="shared" ref="AH36:AH40" si="28">AH34+AF36</f>
-        <v>25990</v>
+        <v>33850</v>
       </c>
       <c r="AI36" s="4">
         <f t="shared" ref="AI36:AI40" si="29">AI34+AG36</f>
-        <v>28680</v>
+        <v>36060</v>
       </c>
       <c r="AJ36" s="4">
         <f>AH36-AI36</f>
-        <v>-2690</v>
+        <v>-2210</v>
       </c>
       <c r="AK36" s="4"/>
       <c r="AL36" s="4"/>
@@ -4562,7 +4581,7 @@
       </c>
       <c r="C37">
         <f t="shared" si="25"/>
-        <v>640</v>
+        <v>770</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>161</v>
@@ -4575,7 +4594,7 @@
       </c>
       <c r="G37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SIEGE_TACTICS" /&gt;&lt;Set Cost="640"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SIEGE_TACTICS" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H37">
         <f t="shared" si="26"/>
@@ -4589,7 +4608,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="27"/>
-        <v>1580</v>
+        <v>2130</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>164</v>
@@ -4602,7 +4621,7 @@
       </c>
       <c r="O37" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CONSERVATION" /&gt;&lt;Set Cost="1580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CONSERVATION" /&gt;&lt;Set Cost="2130"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P37">
         <v>12</v>
@@ -4628,34 +4647,34 @@
         <v>2</v>
       </c>
       <c r="X37">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="Y37">
         <f t="shared" si="19"/>
-        <v>385</v>
+        <v>570</v>
       </c>
       <c r="Z37">
         <f t="shared" si="20"/>
-        <v>2025</v>
+        <v>2760</v>
       </c>
       <c r="AA37">
         <v>120</v>
       </c>
       <c r="AB37">
         <f t="shared" si="23"/>
-        <v>1965</v>
+        <v>2700</v>
       </c>
       <c r="AC37">
         <f t="shared" si="24"/>
-        <v>2085</v>
+        <v>2820</v>
       </c>
       <c r="AD37">
         <f t="shared" si="16"/>
-        <v>4050</v>
+        <v>5520</v>
       </c>
       <c r="AE37">
         <f t="shared" si="17"/>
-        <v>6400</v>
+        <v>8680</v>
       </c>
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
@@ -4675,7 +4694,7 @@
       </c>
       <c r="C38">
         <f t="shared" si="25"/>
-        <v>820</v>
+        <v>1000</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>161</v>
@@ -4688,7 +4707,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_INDUSTRIALIZATION" /&gt;&lt;Set Cost="820"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_INDUSTRIALIZATION" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H38">
         <f t="shared" si="26"/>
@@ -4702,7 +4721,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="27"/>
-        <v>1700</v>
+        <v>2250</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>164</v>
@@ -4715,7 +4734,7 @@
       </c>
       <c r="O38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CAPITALISM" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CAPITALISM" /&gt;&lt;Set Cost="2250"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P38">
         <v>12</v>
@@ -4741,54 +4760,54 @@
         <v>3</v>
       </c>
       <c r="X38">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="Y38">
         <f t="shared" si="19"/>
-        <v>455</v>
+        <v>720</v>
       </c>
       <c r="Z38">
         <f t="shared" si="20"/>
-        <v>2480</v>
+        <v>3480</v>
       </c>
       <c r="AA38">
         <v>160</v>
       </c>
       <c r="AB38">
         <f t="shared" si="23"/>
-        <v>2400</v>
+        <v>3400</v>
       </c>
       <c r="AC38">
         <f t="shared" si="24"/>
-        <v>2560</v>
+        <v>3560</v>
       </c>
       <c r="AD38">
         <f t="shared" si="16"/>
-        <v>7440</v>
+        <v>10440</v>
       </c>
       <c r="AE38">
         <f t="shared" si="17"/>
-        <v>9800</v>
+        <v>13700</v>
       </c>
       <c r="AF38" s="4">
         <f>AD38+AD39</f>
-        <v>13450</v>
+        <v>19140</v>
       </c>
       <c r="AG38" s="4">
         <f>AE38+AE39</f>
-        <v>16940</v>
+        <v>23930</v>
       </c>
       <c r="AH38" s="4">
         <f t="shared" si="28"/>
-        <v>39440</v>
+        <v>52990</v>
       </c>
       <c r="AI38" s="4">
         <f t="shared" si="29"/>
-        <v>45620</v>
+        <v>59990</v>
       </c>
       <c r="AJ38" s="4">
         <f t="shared" ref="AJ38:AJ42" si="30">AH38-AI38</f>
-        <v>-6180</v>
+        <v>-7000</v>
       </c>
       <c r="AK38" s="4"/>
       <c r="AL38" s="4"/>
@@ -4803,7 +4822,7 @@
       </c>
       <c r="C39">
         <f t="shared" si="25"/>
-        <v>820</v>
+        <v>1000</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>161</v>
@@ -4816,7 +4835,7 @@
       </c>
       <c r="G39" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SCIENTIFIC_THEORY" /&gt;&lt;Set Cost="820"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SCIENTIFIC_THEORY" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H39">
         <f t="shared" si="26"/>
@@ -4830,7 +4849,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="27"/>
-        <v>2085</v>
+        <v>2820</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>164</v>
@@ -4843,7 +4862,7 @@
       </c>
       <c r="O39" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NUCLEAR_PROGRAM" /&gt;&lt;Set Cost="2085"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NUCLEAR_PROGRAM" /&gt;&lt;Set Cost="2820"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P39">
         <v>13</v>
@@ -4870,34 +4889,34 @@
         <v>2</v>
       </c>
       <c r="X39">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="Y39">
         <f t="shared" si="19"/>
-        <v>525</v>
+        <v>870</v>
       </c>
       <c r="Z39">
         <f t="shared" si="20"/>
-        <v>3005</v>
+        <v>4350</v>
       </c>
       <c r="AA39">
         <v>0</v>
       </c>
       <c r="AB39">
         <f t="shared" si="23"/>
-        <v>3005</v>
+        <v>4350</v>
       </c>
       <c r="AC39">
         <f t="shared" si="24"/>
-        <v>3005</v>
+        <v>4350</v>
       </c>
       <c r="AD39">
         <f t="shared" si="16"/>
-        <v>6010</v>
+        <v>8700</v>
       </c>
       <c r="AE39">
         <f t="shared" si="17"/>
-        <v>7140</v>
+        <v>10230</v>
       </c>
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
@@ -4917,7 +4936,7 @@
       </c>
       <c r="C40">
         <f t="shared" si="25"/>
-        <v>820</v>
+        <v>1000</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>161</v>
@@ -4930,7 +4949,7 @@
       </c>
       <c r="G40" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BALLISTICS" /&gt;&lt;Set Cost="820"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BALLISTICS" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H40">
         <f t="shared" si="26"/>
@@ -4944,7 +4963,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="27"/>
-        <v>1580</v>
+        <v>2130</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>164</v>
@@ -4957,7 +4976,7 @@
       </c>
       <c r="O40" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MASS_MEDIA" /&gt;&lt;Set Cost="1580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MASS_MEDIA" /&gt;&lt;Set Cost="2130"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P40">
         <v>12</v>
@@ -4984,56 +5003,58 @@
         <v>3</v>
       </c>
       <c r="X40">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="Y40">
         <f t="shared" si="19"/>
-        <v>595</v>
+        <v>1020</v>
       </c>
       <c r="Z40">
         <f t="shared" si="20"/>
-        <v>3600</v>
+        <v>5370</v>
       </c>
       <c r="AA40">
         <v>0</v>
       </c>
       <c r="AB40">
         <f t="shared" si="23"/>
-        <v>3600</v>
+        <v>5370</v>
       </c>
       <c r="AC40">
         <f t="shared" si="24"/>
-        <v>3600</v>
+        <v>5370</v>
       </c>
       <c r="AD40">
         <f t="shared" si="16"/>
-        <v>10800</v>
+        <v>16110</v>
       </c>
       <c r="AE40">
         <f t="shared" si="17"/>
-        <v>17160</v>
+        <v>25200</v>
       </c>
       <c r="AF40" s="4">
         <f>AD40+AD41</f>
-        <v>15491.5</v>
+        <v>23359</v>
       </c>
       <c r="AG40" s="4">
         <f>AE40+AE41</f>
-        <v>27360</v>
+        <v>40530</v>
       </c>
       <c r="AH40" s="4">
         <f t="shared" si="28"/>
-        <v>54931.5</v>
+        <v>76349</v>
       </c>
       <c r="AI40" s="4">
         <f t="shared" si="29"/>
-        <v>72980</v>
+        <v>100520</v>
       </c>
       <c r="AJ40" s="4">
         <f t="shared" si="30"/>
-        <v>-18048.5</v>
-      </c>
-      <c r="AK40" s="4"/>
+        <v>-24171</v>
+      </c>
+      <c r="AK40" s="5" t="s">
+        <v>166</v>
+      </c>
       <c r="AL40" s="4"/>
       <c r="AM40" s="4"/>
     </row>
@@ -5046,7 +5067,7 @@
       </c>
       <c r="C41">
         <f t="shared" si="25"/>
-        <v>820</v>
+        <v>1000</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>161</v>
@@ -5059,7 +5080,7 @@
       </c>
       <c r="G41" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_SCIENCE" /&gt;&lt;Set Cost="820"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_SCIENCE" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H41">
         <f t="shared" si="26"/>
@@ -5073,7 +5094,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="27"/>
-        <v>1580</v>
+        <v>2130</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>164</v>
@@ -5086,7 +5107,7 @@
       </c>
       <c r="O41" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MOBILIZATION" /&gt;&lt;Set Cost="1580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MOBILIZATION" /&gt;&lt;Set Cost="2130"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P41">
         <v>12</v>
@@ -5112,41 +5133,41 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X41">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="Y41">
         <f t="shared" si="19"/>
-        <v>665</v>
+        <v>1220</v>
       </c>
       <c r="Z41">
         <f t="shared" si="20"/>
-        <v>4265</v>
+        <v>6590</v>
       </c>
       <c r="AA41">
         <v>0</v>
       </c>
       <c r="AB41">
         <f t="shared" si="23"/>
-        <v>4265</v>
+        <v>6590</v>
       </c>
       <c r="AC41">
         <f t="shared" si="24"/>
-        <v>4265</v>
+        <v>6590</v>
       </c>
       <c r="AD41">
         <f t="shared" si="16"/>
-        <v>4691.5</v>
+        <v>7249.0000000000009</v>
       </c>
       <c r="AE41">
         <f t="shared" si="17"/>
-        <v>10200</v>
+        <v>15330</v>
       </c>
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
       <c r="AH41" s="4"/>
       <c r="AI41" s="4"/>
       <c r="AJ41" s="4"/>
-      <c r="AK41" s="4"/>
+      <c r="AK41" s="5"/>
       <c r="AL41" s="4"/>
       <c r="AM41" s="4"/>
     </row>
@@ -5159,7 +5180,7 @@
       </c>
       <c r="C42">
         <f t="shared" si="25"/>
-        <v>1040</v>
+        <v>1310</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>161</v>
@@ -5172,7 +5193,7 @@
       </c>
       <c r="G42" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEAM_POWER" /&gt;&lt;Set Cost="1040"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEAM_POWER" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H42">
         <f t="shared" si="26"/>
@@ -5186,7 +5207,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="27"/>
-        <v>1965</v>
+        <v>2700</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>164</v>
@@ -5199,7 +5220,7 @@
       </c>
       <c r="O42" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_IDEOLOGY" /&gt;&lt;Set Cost="1965"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_IDEOLOGY" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P42">
         <v>13</v>
@@ -5225,56 +5246,59 @@
         <v>1</v>
       </c>
       <c r="X42">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="Y42">
         <f t="shared" si="19"/>
-        <v>745</v>
+        <v>1420</v>
       </c>
       <c r="Z42">
         <f t="shared" si="20"/>
-        <v>5010</v>
+        <v>8010</v>
       </c>
       <c r="AA42">
         <v>0</v>
       </c>
       <c r="AB42">
         <f t="shared" si="23"/>
-        <v>5010</v>
+        <v>8010</v>
       </c>
       <c r="AC42">
         <f t="shared" si="24"/>
-        <v>5010</v>
+        <v>8010</v>
       </c>
       <c r="AD42">
         <f t="shared" si="16"/>
-        <v>5010</v>
+        <v>8010</v>
       </c>
       <c r="AE42">
         <f t="shared" si="17"/>
-        <v>24120</v>
+        <v>36960</v>
       </c>
       <c r="AF42" s="4">
         <f>AD42+AD43</f>
-        <v>28350</v>
+        <v>46530</v>
       </c>
       <c r="AG42" s="4">
         <f>AE42+AE43</f>
-        <v>28840</v>
+        <v>44310</v>
       </c>
       <c r="AH42" s="4">
         <f t="shared" ref="AH42:AI42" si="31">AH40+AF42</f>
-        <v>83281.5</v>
+        <v>122879</v>
       </c>
       <c r="AI42" s="4">
         <f t="shared" si="31"/>
-        <v>101820</v>
+        <v>144830</v>
       </c>
       <c r="AJ42" s="4">
         <f t="shared" si="30"/>
-        <v>-18538.5</v>
-      </c>
-      <c r="AK42" s="4"/>
+        <v>-21951</v>
+      </c>
+      <c r="AK42" s="4">
+        <f>Z43+0.5*Y44</f>
+        <v>10065</v>
+      </c>
       <c r="AL42" s="4"/>
       <c r="AM42" s="4"/>
     </row>
@@ -5287,7 +5311,7 @@
       </c>
       <c r="C43">
         <f t="shared" si="25"/>
-        <v>1040</v>
+        <v>1310</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>161</v>
@@ -5300,7 +5324,7 @@
       </c>
       <c r="G43" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SANITATION" /&gt;&lt;Set Cost="1040"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SANITATION" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H43">
         <f t="shared" si="26"/>
@@ -5314,7 +5338,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="27"/>
-        <v>1965</v>
+        <v>2700</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>164</v>
@@ -5327,7 +5351,7 @@
       </c>
       <c r="O43" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SUFFRAGE" /&gt;&lt;Set Cost="1965"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SUFFRAGE" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P43">
         <v>13</v>
@@ -5354,34 +5378,34 @@
         <v>4</v>
       </c>
       <c r="X43">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="Y43">
         <f t="shared" si="19"/>
-        <v>825</v>
+        <v>1620</v>
       </c>
       <c r="Z43">
         <f t="shared" si="20"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="AA43">
         <v>0</v>
       </c>
       <c r="AB43">
         <f t="shared" si="23"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="AC43">
         <f t="shared" si="24"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="AD43">
         <f t="shared" si="16"/>
-        <v>23340</v>
+        <v>38520</v>
       </c>
       <c r="AE43">
         <f t="shared" si="17"/>
-        <v>4720</v>
+        <v>7350</v>
       </c>
       <c r="AF43" s="4"/>
       <c r="AG43" s="4"/>
@@ -5401,7 +5425,7 @@
       </c>
       <c r="C44">
         <f t="shared" si="25"/>
-        <v>1040</v>
+        <v>1310</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>161</v>
@@ -5414,7 +5438,7 @@
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ECONOMICS" /&gt;&lt;Set Cost="1040"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ECONOMICS" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H44">
         <f t="shared" si="26"/>
@@ -5428,7 +5452,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="27"/>
-        <v>1965</v>
+        <v>2700</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>164</v>
@@ -5441,7 +5465,7 @@
       </c>
       <c r="O44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_TOTALITARIANISM" /&gt;&lt;Set Cost="1965"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_TOTALITARIANISM" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P44">
         <v>13</v>
@@ -5467,54 +5491,54 @@
         <v>1</v>
       </c>
       <c r="X44">
-        <v>80</v>
+        <v>-750</v>
       </c>
       <c r="Y44">
         <f>Y43+X44</f>
-        <v>905</v>
+        <v>870</v>
       </c>
       <c r="Z44">
         <f>Z43+Y44</f>
-        <v>6740</v>
+        <v>10500</v>
       </c>
       <c r="AA44">
         <v>0</v>
       </c>
       <c r="AB44">
         <f t="shared" si="23"/>
-        <v>6740</v>
+        <v>10500</v>
       </c>
       <c r="AC44">
         <f t="shared" si="24"/>
-        <v>6740</v>
+        <v>10500</v>
       </c>
       <c r="AD44">
         <f t="shared" si="16"/>
-        <v>6740</v>
+        <v>10500</v>
       </c>
       <c r="AE44">
         <f t="shared" si="17"/>
-        <v>5500</v>
+        <v>8000</v>
       </c>
       <c r="AF44" s="2">
         <f>AD44</f>
-        <v>6740</v>
+        <v>10500</v>
       </c>
       <c r="AG44" s="2">
         <f>AE44</f>
-        <v>5500</v>
+        <v>8000</v>
       </c>
       <c r="AH44">
         <f t="shared" ref="AH44:AI44" si="32">AH42+AF44</f>
-        <v>90021.5</v>
+        <v>133379</v>
       </c>
       <c r="AI44">
         <f t="shared" si="32"/>
-        <v>107320</v>
+        <v>152830</v>
       </c>
       <c r="AJ44">
         <f>AH44-AI44</f>
-        <v>-17298.5</v>
+        <v>-19451</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
@@ -5526,7 +5550,7 @@
       </c>
       <c r="C45">
         <f t="shared" si="25"/>
-        <v>1040</v>
+        <v>1310</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>161</v>
@@ -5539,7 +5563,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RIFLING" /&gt;&lt;Set Cost="1040"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RIFLING" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H45">
         <f t="shared" si="26"/>
@@ -5553,7 +5577,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="27"/>
-        <v>1965</v>
+        <v>2700</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>164</v>
@@ -5566,7 +5590,7 @@
       </c>
       <c r="O45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CLASS_STRUGGLE" /&gt;&lt;Set Cost="1965"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CLASS_STRUGGLE" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P45">
         <v>13</v>
@@ -5581,7 +5605,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="25"/>
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>161</v>
@@ -5594,7 +5618,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FLIGHT" /&gt;&lt;Set Cost="1300"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FLIGHT" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H46">
         <f t="shared" si="26"/>
@@ -5608,7 +5632,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="27"/>
-        <v>2560</v>
+        <v>3560</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>164</v>
@@ -5621,7 +5645,7 @@
       </c>
       <c r="O46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLD_WAR" /&gt;&lt;Set Cost="2560"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLD_WAR" /&gt;&lt;Set Cost="3560"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P46">
         <v>14</v>
@@ -5631,7 +5655,7 @@
       </c>
       <c r="T46">
         <f>AB25</f>
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
@@ -5643,7 +5667,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="25"/>
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>161</v>
@@ -5656,7 +5680,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REPLACEABLE_PARTS" /&gt;&lt;Set Cost="1300"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REPLACEABLE_PARTS" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H47">
         <f t="shared" si="26"/>
@@ -5670,7 +5694,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="27"/>
-        <v>2560</v>
+        <v>3560</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>164</v>
@@ -5683,7 +5707,7 @@
       </c>
       <c r="O47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_PROFESSIONAL_SPORTS" /&gt;&lt;Set Cost="2560"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_PROFESSIONAL_SPORTS" /&gt;&lt;Set Cost="3560"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P47">
         <v>14</v>
@@ -5693,7 +5717,7 @@
       </c>
       <c r="T47">
         <f>AB26</f>
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
@@ -5705,7 +5729,7 @@
       </c>
       <c r="C48">
         <f t="shared" si="25"/>
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>161</v>
@@ -5718,7 +5742,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEEL" /&gt;&lt;Set Cost="1300"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEEL" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H48">
         <f t="shared" si="26"/>
@@ -5732,7 +5756,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="27"/>
-        <v>2400</v>
+        <v>3400</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>164</v>
@@ -5745,7 +5769,7 @@
       </c>
       <c r="O48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HERITAGE" /&gt;&lt;Set Cost="2400"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HERITAGE" /&gt;&lt;Set Cost="3400"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P48">
         <v>14</v>
@@ -5755,7 +5779,7 @@
       </c>
       <c r="T48">
         <f>AB27</f>
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
@@ -5767,7 +5791,7 @@
       </c>
       <c r="C49">
         <f t="shared" si="25"/>
-        <v>1600</v>
+        <v>2170</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>161</v>
@@ -5780,7 +5804,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ELECTRICITY" /&gt;&lt;Set Cost="1600"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ELECTRICITY" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H49">
         <f t="shared" si="26"/>
@@ -5794,7 +5818,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="27"/>
-        <v>3005</v>
+        <v>4350</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>164</v>
@@ -5807,7 +5831,7 @@
       </c>
       <c r="O49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RAPID_DEPLOYMENT" /&gt;&lt;Set Cost="3005"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RAPID_DEPLOYMENT" /&gt;&lt;Set Cost="4350"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P49">
         <v>15</v>
@@ -5817,7 +5841,7 @@
       </c>
       <c r="T49">
         <f>AC27</f>
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
@@ -5829,7 +5853,7 @@
       </c>
       <c r="C50">
         <f t="shared" si="25"/>
-        <v>1600</v>
+        <v>2170</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>161</v>
@@ -5842,7 +5866,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RADIO" /&gt;&lt;Set Cost="1600"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RADIO" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H50">
         <f t="shared" si="26"/>
@@ -5856,7 +5880,7 @@
       </c>
       <c r="K50">
         <f t="shared" si="27"/>
-        <v>3005</v>
+        <v>4350</v>
       </c>
       <c r="L50" s="3" t="s">
         <v>164</v>
@@ -5869,7 +5893,7 @@
       </c>
       <c r="O50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SPACE_RACE" /&gt;&lt;Set Cost="3005"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SPACE_RACE" /&gt;&lt;Set Cost="4350"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P50">
         <v>15</v>
@@ -5879,7 +5903,7 @@
       </c>
       <c r="T50">
         <f>AB28</f>
-        <v>160</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
@@ -5891,7 +5915,7 @@
       </c>
       <c r="C51">
         <f t="shared" si="25"/>
-        <v>1600</v>
+        <v>2170</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>161</v>
@@ -5904,7 +5928,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CHEMISTRY" /&gt;&lt;Set Cost="1600"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CHEMISTRY" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H51">
         <f t="shared" si="26"/>
@@ -5918,7 +5942,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="27"/>
-        <v>3600</v>
+        <v>5370</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>164</v>
@@ -5931,7 +5955,7 @@
       </c>
       <c r="O51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBALIZATION" /&gt;&lt;Set Cost="3600"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBALIZATION" /&gt;&lt;Set Cost="5370"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P51">
         <v>16</v>
@@ -5941,7 +5965,7 @@
       </c>
       <c r="T51">
         <f>AB29</f>
-        <v>195</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
@@ -5953,7 +5977,7 @@
       </c>
       <c r="C52">
         <f t="shared" si="25"/>
-        <v>1600</v>
+        <v>2170</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>161</v>
@@ -5966,7 +5990,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBUSTION" /&gt;&lt;Set Cost="1600"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBUSTION" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H52">
         <f t="shared" si="26"/>
@@ -5980,7 +6004,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="27"/>
-        <v>3600</v>
+        <v>5370</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>164</v>
@@ -5993,7 +6017,7 @@
       </c>
       <c r="O52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SOCIAL_MEDIA" /&gt;&lt;Set Cost="3600"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SOCIAL_MEDIA" /&gt;&lt;Set Cost="5370"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P52">
         <v>16</v>
@@ -6003,7 +6027,7 @@
       </c>
       <c r="T52">
         <f>AC29</f>
-        <v>255</v>
+        <v>310</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -6015,7 +6039,7 @@
       </c>
       <c r="C53">
         <f t="shared" si="25"/>
-        <v>1960</v>
+        <v>2740</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>161</v>
@@ -6028,7 +6052,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_FLIGHT" /&gt;&lt;Set Cost="1960"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_FLIGHT" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H53">
         <f t="shared" si="26"/>
@@ -6042,7 +6066,7 @@
       </c>
       <c r="K53">
         <f t="shared" si="27"/>
-        <v>6740</v>
+        <v>10500</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>164</v>
@@ -6055,7 +6079,7 @@
       </c>
       <c r="O53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FUTURE_CIVIC" /&gt;&lt;Set Cost="6740"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FUTURE_CIVIC" /&gt;&lt;Set Cost="10500"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P53">
         <v>20</v>
@@ -6065,7 +6089,7 @@
       </c>
       <c r="T53">
         <f>AB30</f>
-        <v>275</v>
+        <v>355</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
@@ -6077,7 +6101,7 @@
       </c>
       <c r="C54">
         <f t="shared" si="25"/>
-        <v>1960</v>
+        <v>2740</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>161</v>
@@ -6090,7 +6114,7 @@
       </c>
       <c r="G54" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROCKETRY" /&gt;&lt;Set Cost="1960"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROCKETRY" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H54">
         <f t="shared" si="26"/>
@@ -6104,7 +6128,7 @@
       </c>
       <c r="K54">
         <f t="shared" si="27"/>
-        <v>3600</v>
+        <v>5370</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>164</v>
@@ -6117,7 +6141,7 @@
       </c>
       <c r="O54" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_ENVIRONMENTALISM" /&gt;&lt;Set Cost="3600"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_ENVIRONMENTALISM" /&gt;&lt;Set Cost="5370"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P54">
         <v>16</v>
@@ -6127,7 +6151,7 @@
       </c>
       <c r="T54">
         <f>AC30</f>
-        <v>365</v>
+        <v>445</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
@@ -6139,7 +6163,7 @@
       </c>
       <c r="C55">
         <f t="shared" si="25"/>
-        <v>1960</v>
+        <v>2740</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>161</v>
@@ -6152,7 +6176,7 @@
       </c>
       <c r="G55" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_BALLISTICS" /&gt;&lt;Set Cost="1960"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_BALLISTICS" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H55">
         <f t="shared" si="26"/>
@@ -6166,7 +6190,7 @@
       </c>
       <c r="K55">
         <f t="shared" si="27"/>
-        <v>4265</v>
+        <v>6590</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>164</v>
@@ -6179,7 +6203,7 @@
       </c>
       <c r="O55" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CORPORATE_LIBERTARIANISM" /&gt;&lt;Set Cost="4265"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CORPORATE_LIBERTARIANISM" /&gt;&lt;Set Cost="6590"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P55">
         <v>17</v>
@@ -6189,7 +6213,7 @@
       </c>
       <c r="T55">
         <f>AB31</f>
-        <v>400</v>
+        <v>505</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
@@ -6201,7 +6225,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="25"/>
-        <v>1960</v>
+        <v>2740</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>161</v>
@@ -6214,7 +6238,7 @@
       </c>
       <c r="G56" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBINED_ARMS" /&gt;&lt;Set Cost="1960"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBINED_ARMS" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H56">
         <f t="shared" si="26"/>
@@ -6228,7 +6252,7 @@
       </c>
       <c r="K56">
         <f t="shared" si="27"/>
-        <v>4265</v>
+        <v>6590</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>164</v>
@@ -6241,7 +6265,7 @@
       </c>
       <c r="O56" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIGITAL_DEMOCRACY" /&gt;&lt;Set Cost="4265"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIGITAL_DEMOCRACY" /&gt;&lt;Set Cost="6590"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P56">
         <v>17</v>
@@ -6251,7 +6275,7 @@
       </c>
       <c r="T56">
         <f>AC31</f>
-        <v>490</v>
+        <v>595</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
@@ -6263,7 +6287,7 @@
       </c>
       <c r="C57">
         <f t="shared" si="25"/>
-        <v>1960</v>
+        <v>2740</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>161</v>
@@ -6276,7 +6300,7 @@
       </c>
       <c r="G57" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PLASTICS" /&gt;&lt;Set Cost="1960"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PLASTICS" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H57">
         <f t="shared" si="26"/>
@@ -6290,7 +6314,7 @@
       </c>
       <c r="K57">
         <f t="shared" si="27"/>
-        <v>4265</v>
+        <v>6590</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>164</v>
@@ -6303,7 +6327,7 @@
       </c>
       <c r="O57" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SYNTHETIC_TECHNOCRACY" /&gt;&lt;Set Cost="4265"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SYNTHETIC_TECHNOCRACY" /&gt;&lt;Set Cost="6590"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P57">
         <v>17</v>
@@ -6313,7 +6337,7 @@
       </c>
       <c r="T57">
         <f>AB32</f>
-        <v>540</v>
+        <v>690</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
@@ -6325,7 +6349,7 @@
       </c>
       <c r="C58">
         <f t="shared" si="25"/>
-        <v>2380</v>
+        <v>3410</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>161</v>
@@ -6338,7 +6362,7 @@
       </c>
       <c r="G58" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPUTERS" /&gt;&lt;Set Cost="2380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPUTERS" /&gt;&lt;Set Cost="3410"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H58">
         <f t="shared" si="26"/>
@@ -6352,7 +6376,7 @@
       </c>
       <c r="K58">
         <f t="shared" si="27"/>
-        <v>5010</v>
+        <v>8010</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>164</v>
@@ -6365,7 +6389,7 @@
       </c>
       <c r="O58" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NEAR_FUTURE_GOVERNANCE" /&gt;&lt;Set Cost="5010"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NEAR_FUTURE_GOVERNANCE" /&gt;&lt;Set Cost="8010"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P58">
         <v>17</v>
@@ -6375,7 +6399,7 @@
       </c>
       <c r="T58">
         <f>AC32</f>
-        <v>660</v>
+        <v>810</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
@@ -6387,7 +6411,7 @@
       </c>
       <c r="C59">
         <f t="shared" si="25"/>
-        <v>2380</v>
+        <v>3410</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>161</v>
@@ -6400,7 +6424,7 @@
       </c>
       <c r="G59" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FISSION" /&gt;&lt;Set Cost="2380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FISSION" /&gt;&lt;Set Cost="3410"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H59">
         <f t="shared" si="26"/>
@@ -6414,7 +6438,7 @@
       </c>
       <c r="K59">
         <f t="shared" si="27"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>164</v>
@@ -6427,7 +6451,7 @@
       </c>
       <c r="O59" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBAL_WARMING_MITIGATION" /&gt;&lt;Set Cost="5835"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBAL_WARMING_MITIGATION" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P59">
         <v>18</v>
@@ -6437,7 +6461,7 @@
       </c>
       <c r="T59">
         <f>AB33</f>
-        <v>785</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
@@ -6449,7 +6473,7 @@
       </c>
       <c r="C60">
         <f t="shared" si="25"/>
-        <v>2380</v>
+        <v>3410</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>161</v>
@@ -6462,7 +6486,7 @@
       </c>
       <c r="G60" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SYNTHETIC_MATERIALS" /&gt;&lt;Set Cost="2380"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SYNTHETIC_MATERIALS" /&gt;&lt;Set Cost="3410"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H60">
         <f t="shared" si="26"/>
@@ -6476,7 +6500,7 @@
       </c>
       <c r="K60">
         <f t="shared" si="27"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>164</v>
@@ -6489,7 +6513,7 @@
       </c>
       <c r="O60" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SMART_POWER_DOCTRINE" /&gt;&lt;Set Cost="5835"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SMART_POWER_DOCTRINE" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P60">
         <v>19</v>
@@ -6499,7 +6523,7 @@
       </c>
       <c r="T60">
         <f>AB34</f>
-        <v>945</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
@@ -6511,7 +6535,7 @@
       </c>
       <c r="C61">
         <f t="shared" si="25"/>
-        <v>2860</v>
+        <v>4200</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>161</v>
@@ -6524,7 +6548,7 @@
       </c>
       <c r="G61" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_TELECOMMUNICATIONS" /&gt;&lt;Set Cost="2860"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_TELECOMMUNICATIONS" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H61">
         <f t="shared" si="26"/>
@@ -6538,7 +6562,7 @@
       </c>
       <c r="K61">
         <f t="shared" si="27"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>164</v>
@@ -6551,7 +6575,7 @@
       </c>
       <c r="O61" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_INFORMATION_WARFARE" /&gt;&lt;Set Cost="5835"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_INFORMATION_WARFARE" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P61">
         <v>19</v>
@@ -6561,7 +6585,7 @@
       </c>
       <c r="T61">
         <f>AC34</f>
-        <v>1095</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
@@ -6573,7 +6597,7 @@
       </c>
       <c r="C62">
         <f t="shared" si="25"/>
-        <v>2860</v>
+        <v>4200</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>161</v>
@@ -6586,7 +6610,7 @@
       </c>
       <c r="G62" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SATELLITES" /&gt;&lt;Set Cost="2860"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SATELLITES" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H62">
         <f t="shared" si="26"/>
@@ -6600,7 +6624,7 @@
       </c>
       <c r="K62">
         <f t="shared" si="27"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>164</v>
@@ -6613,7 +6637,7 @@
       </c>
       <c r="O62" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXODUS_IMPERATIVE" /&gt;&lt;Set Cost="5835"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXODUS_IMPERATIVE" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P62">
         <v>19</v>
@@ -6623,7 +6647,7 @@
       </c>
       <c r="T62">
         <f>AB35</f>
-        <v>1230</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
@@ -6635,7 +6659,7 @@
       </c>
       <c r="C63">
         <f t="shared" si="25"/>
-        <v>2860</v>
+        <v>4200</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>161</v>
@@ -6648,7 +6672,7 @@
       </c>
       <c r="G63" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUIDANCE_SYSTEMS" /&gt;&lt;Set Cost="2860"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUIDANCE_SYSTEMS" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H63">
         <f t="shared" si="26"/>
@@ -6662,7 +6686,7 @@
       </c>
       <c r="K63">
         <f t="shared" si="27"/>
-        <v>5835</v>
+        <v>9630</v>
       </c>
       <c r="L63" s="3" t="s">
         <v>164</v>
@@ -6675,7 +6699,7 @@
       </c>
       <c r="O63" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HEGEMONY" /&gt;&lt;Set Cost="5835"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HEGEMONY" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P63">
         <v>19</v>
@@ -6685,7 +6709,7 @@
       </c>
       <c r="T63">
         <f>AC35</f>
-        <v>1380</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
@@ -6697,7 +6721,7 @@
       </c>
       <c r="C64">
         <f t="shared" si="25"/>
-        <v>2860</v>
+        <v>4200</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>161</v>
@@ -6710,7 +6734,7 @@
       </c>
       <c r="G64" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_LASERS" /&gt;&lt;Set Cost="2860"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_LASERS" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H64">
         <f t="shared" si="26"/>
@@ -6725,7 +6749,7 @@
       </c>
       <c r="T64">
         <f>AB36</f>
-        <v>1580</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
@@ -6737,7 +6761,7 @@
       </c>
       <c r="C65">
         <f t="shared" si="25"/>
-        <v>2860</v>
+        <v>4200</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>161</v>
@@ -6750,7 +6774,7 @@
       </c>
       <c r="G65" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPOSITES" /&gt;&lt;Set Cost="2860"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPOSITES" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H65">
         <f t="shared" si="26"/>
@@ -6765,7 +6789,7 @@
       </c>
       <c r="T65">
         <f>AC36</f>
-        <v>1700</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
@@ -6777,7 +6801,7 @@
       </c>
       <c r="C66">
         <f t="shared" si="25"/>
-        <v>2860</v>
+        <v>4200</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>161</v>
@@ -6790,7 +6814,7 @@
       </c>
       <c r="G66" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEALTH_TECHNOLOGY" /&gt;&lt;Set Cost="2860"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEALTH_TECHNOLOGY" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H66">
         <f t="shared" si="26"/>
@@ -6805,7 +6829,7 @@
       </c>
       <c r="T66">
         <f>AB37</f>
-        <v>1965</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
@@ -6817,7 +6841,7 @@
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C79" si="33">VLOOKUP(B67,$T$3:$AB$22,9,FALSE)</f>
-        <v>3400</v>
+        <v>5110</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>161</v>
@@ -6830,7 +6854,7 @@
       </c>
       <c r="G67" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROBOTICS" /&gt;&lt;Set Cost="3400"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROBOTICS" /&gt;&lt;Set Cost="5110"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H79" si="34">VLOOKUP(B67,$T$3:$U$22,2,FALSE)</f>
@@ -6845,7 +6869,7 @@
       </c>
       <c r="T67">
         <f>AC37</f>
-        <v>2085</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
@@ -6857,7 +6881,7 @@
       </c>
       <c r="C68">
         <f t="shared" si="33"/>
-        <v>3400</v>
+        <v>5110</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>161</v>
@@ -6870,7 +6894,7 @@
       </c>
       <c r="G68" s="3" t="str">
         <f t="shared" ref="G68:G79" si="35">_xlfn.CONCAT(D68,A68,E68,C68,F68)</f>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NANOTECHNOLOGY" /&gt;&lt;Set Cost="3400"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NANOTECHNOLOGY" /&gt;&lt;Set Cost="5110"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H68">
         <f t="shared" si="34"/>
@@ -6885,7 +6909,7 @@
       </c>
       <c r="T68">
         <f>AB38</f>
-        <v>2400</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
@@ -6897,7 +6921,7 @@
       </c>
       <c r="C69">
         <f t="shared" si="33"/>
-        <v>3400</v>
+        <v>5110</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>161</v>
@@ -6910,7 +6934,7 @@
       </c>
       <c r="G69" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FUSION" /&gt;&lt;Set Cost="3400"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FUSION" /&gt;&lt;Set Cost="5110"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H69">
         <f t="shared" si="34"/>
@@ -6925,7 +6949,7 @@
       </c>
       <c r="T69">
         <f>AC38</f>
-        <v>2560</v>
+        <v>3560</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
@@ -6937,7 +6961,7 @@
       </c>
       <c r="C70">
         <f t="shared" si="33"/>
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>161</v>
@@ -6950,7 +6974,7 @@
       </c>
       <c r="G70" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BUTTRESS" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BUTTRESS" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H70">
         <f t="shared" si="34"/>
@@ -6964,8 +6988,8 @@
         <v>2415</v>
       </c>
       <c r="T70">
-        <f>AB39</f>
-        <v>3005</v>
+        <f t="shared" ref="T70:T75" si="36">AB39</f>
+        <v>4350</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
@@ -6977,7 +7001,7 @@
       </c>
       <c r="C71">
         <f t="shared" si="33"/>
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>161</v>
@@ -6990,7 +7014,7 @@
       </c>
       <c r="G71" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REFINING" /&gt;&lt;Set Cost="1300"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REFINING" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H71">
         <f t="shared" si="34"/>
@@ -7004,8 +7028,8 @@
         <v>2880</v>
       </c>
       <c r="T71">
-        <f>AB40</f>
-        <v>3600</v>
+        <f t="shared" si="36"/>
+        <v>5370</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
@@ -7017,7 +7041,7 @@
       </c>
       <c r="C72">
         <f t="shared" si="33"/>
-        <v>4020</v>
+        <v>6160</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>161</v>
@@ -7030,7 +7054,7 @@
       </c>
       <c r="G72" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SEASTEADS" /&gt;&lt;Set Cost="4020"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SEASTEADS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H72">
         <f t="shared" si="34"/>
@@ -7044,8 +7068,8 @@
         <v>3000</v>
       </c>
       <c r="T72">
-        <f>AB41</f>
-        <v>4265</v>
+        <f t="shared" si="36"/>
+        <v>6590</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
@@ -7057,7 +7081,7 @@
       </c>
       <c r="C73">
         <f t="shared" si="33"/>
-        <v>4020</v>
+        <v>6160</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>161</v>
@@ -7070,7 +7094,7 @@
       </c>
       <c r="G73" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_AI" /&gt;&lt;Set Cost="4020"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_AI" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H73">
         <f t="shared" si="34"/>
@@ -7084,8 +7108,8 @@
         <v>3100</v>
       </c>
       <c r="T73">
-        <f>AB42</f>
-        <v>5010</v>
+        <f t="shared" si="36"/>
+        <v>8010</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
@@ -7097,7 +7121,7 @@
       </c>
       <c r="C74">
         <f t="shared" si="33"/>
-        <v>4020</v>
+        <v>6160</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>161</v>
@@ -7110,7 +7134,7 @@
       </c>
       <c r="G74" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_POWER_CELLS" /&gt;&lt;Set Cost="4020"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_POWER_CELLS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H74">
         <f t="shared" si="34"/>
@@ -7124,8 +7148,8 @@
         <v>3200</v>
       </c>
       <c r="T74">
-        <f>AB43</f>
-        <v>5835</v>
+        <f t="shared" si="36"/>
+        <v>9630</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
@@ -7137,7 +7161,7 @@
       </c>
       <c r="C75">
         <f t="shared" si="33"/>
-        <v>4020</v>
+        <v>6160</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>161</v>
@@ -7150,7 +7174,7 @@
       </c>
       <c r="G75" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CYBERNETICS" /&gt;&lt;Set Cost="4020"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CYBERNETICS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H75">
         <f t="shared" si="34"/>
@@ -7164,8 +7188,8 @@
         <v>3500</v>
       </c>
       <c r="T75">
-        <f>AB44</f>
-        <v>6740</v>
+        <f t="shared" si="36"/>
+        <v>10500</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
@@ -7177,7 +7201,7 @@
       </c>
       <c r="C76">
         <f t="shared" si="33"/>
-        <v>4020</v>
+        <v>6160</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>161</v>
@@ -7190,7 +7214,7 @@
       </c>
       <c r="G76" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SMART_MATERIALS" /&gt;&lt;Set Cost="4020"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SMART_MATERIALS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H76">
         <f t="shared" si="34"/>
@@ -7210,7 +7234,7 @@
       </c>
       <c r="C77">
         <f t="shared" si="33"/>
-        <v>4020</v>
+        <v>6160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>161</v>
@@ -7223,7 +7247,7 @@
       </c>
       <c r="G77" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PREDICTIVE_SYSTEMS" /&gt;&lt;Set Cost="4020"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PREDICTIVE_SYSTEMS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H77">
         <f t="shared" si="34"/>
@@ -7243,7 +7267,7 @@
       </c>
       <c r="C78">
         <f t="shared" si="33"/>
-        <v>4720</v>
+        <v>7350</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>161</v>
@@ -7256,7 +7280,7 @@
       </c>
       <c r="G78" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_OFFWORLD_MISSION" /&gt;&lt;Set Cost="4720"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_OFFWORLD_MISSION" /&gt;&lt;Set Cost="7350"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H78">
         <f t="shared" si="34"/>
@@ -7276,7 +7300,7 @@
       </c>
       <c r="C79">
         <f t="shared" si="33"/>
-        <v>5500</v>
+        <v>8000</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>161</v>
@@ -7289,7 +7313,7 @@
       </c>
       <c r="G79" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FUTURE_TECH" /&gt;&lt;Set Cost="5500"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FUTURE_TECH" /&gt;&lt;Set Cost="8000"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H79">
         <f t="shared" si="34"/>
@@ -7302,6 +7326,63 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="AF42:AF43"/>
+    <mergeCell ref="AG25:AG27"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="AG30:AG31"/>
+    <mergeCell ref="AG32:AG33"/>
+    <mergeCell ref="AG34:AG35"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="AG38:AG39"/>
+    <mergeCell ref="AG40:AG41"/>
+    <mergeCell ref="AG42:AG43"/>
+    <mergeCell ref="AF25:AF27"/>
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AF30:AF31"/>
+    <mergeCell ref="AF32:AF33"/>
+    <mergeCell ref="AF34:AF35"/>
+    <mergeCell ref="AF36:AF37"/>
+    <mergeCell ref="AF38:AF39"/>
+    <mergeCell ref="AF40:AF41"/>
+    <mergeCell ref="AH36:AH37"/>
+    <mergeCell ref="AH38:AH39"/>
+    <mergeCell ref="AH40:AH41"/>
+    <mergeCell ref="AH42:AH43"/>
+    <mergeCell ref="AI25:AI27"/>
+    <mergeCell ref="AI28:AI29"/>
+    <mergeCell ref="AI30:AI31"/>
+    <mergeCell ref="AI32:AI33"/>
+    <mergeCell ref="AI34:AI35"/>
+    <mergeCell ref="AI36:AI37"/>
+    <mergeCell ref="AI38:AI39"/>
+    <mergeCell ref="AI40:AI41"/>
+    <mergeCell ref="AI42:AI43"/>
+    <mergeCell ref="AH25:AH27"/>
+    <mergeCell ref="AH28:AH29"/>
+    <mergeCell ref="AH30:AH31"/>
+    <mergeCell ref="AH32:AH33"/>
+    <mergeCell ref="AH34:AH35"/>
+    <mergeCell ref="AJ42:AJ43"/>
+    <mergeCell ref="AK25:AK27"/>
+    <mergeCell ref="AK28:AK29"/>
+    <mergeCell ref="AK30:AK31"/>
+    <mergeCell ref="AK32:AK33"/>
+    <mergeCell ref="AK34:AK35"/>
+    <mergeCell ref="AK36:AK37"/>
+    <mergeCell ref="AK38:AK39"/>
+    <mergeCell ref="AK40:AK41"/>
+    <mergeCell ref="AK42:AK43"/>
+    <mergeCell ref="AJ25:AJ27"/>
+    <mergeCell ref="AJ28:AJ29"/>
+    <mergeCell ref="AJ30:AJ31"/>
+    <mergeCell ref="AJ32:AJ33"/>
+    <mergeCell ref="AJ34:AJ35"/>
+    <mergeCell ref="AJ36:AJ37"/>
+    <mergeCell ref="AJ38:AJ39"/>
+    <mergeCell ref="AJ40:AJ41"/>
+    <mergeCell ref="AL36:AL37"/>
+    <mergeCell ref="AL38:AL39"/>
+    <mergeCell ref="AL40:AL41"/>
     <mergeCell ref="AL42:AL43"/>
     <mergeCell ref="AM25:AM27"/>
     <mergeCell ref="AM28:AM29"/>
@@ -7317,63 +7398,6 @@
     <mergeCell ref="AL30:AL31"/>
     <mergeCell ref="AL32:AL33"/>
     <mergeCell ref="AL34:AL35"/>
-    <mergeCell ref="AJ36:AJ37"/>
-    <mergeCell ref="AJ38:AJ39"/>
-    <mergeCell ref="AJ40:AJ41"/>
-    <mergeCell ref="AL36:AL37"/>
-    <mergeCell ref="AL38:AL39"/>
-    <mergeCell ref="AL40:AL41"/>
-    <mergeCell ref="AJ42:AJ43"/>
-    <mergeCell ref="AK25:AK27"/>
-    <mergeCell ref="AK28:AK29"/>
-    <mergeCell ref="AK30:AK31"/>
-    <mergeCell ref="AK32:AK33"/>
-    <mergeCell ref="AK34:AK35"/>
-    <mergeCell ref="AK36:AK37"/>
-    <mergeCell ref="AK38:AK39"/>
-    <mergeCell ref="AK40:AK41"/>
-    <mergeCell ref="AK42:AK43"/>
-    <mergeCell ref="AJ25:AJ27"/>
-    <mergeCell ref="AJ28:AJ29"/>
-    <mergeCell ref="AJ30:AJ31"/>
-    <mergeCell ref="AJ32:AJ33"/>
-    <mergeCell ref="AJ34:AJ35"/>
-    <mergeCell ref="AH42:AH43"/>
-    <mergeCell ref="AI25:AI27"/>
-    <mergeCell ref="AI28:AI29"/>
-    <mergeCell ref="AI30:AI31"/>
-    <mergeCell ref="AI32:AI33"/>
-    <mergeCell ref="AI34:AI35"/>
-    <mergeCell ref="AI36:AI37"/>
-    <mergeCell ref="AI38:AI39"/>
-    <mergeCell ref="AI40:AI41"/>
-    <mergeCell ref="AI42:AI43"/>
-    <mergeCell ref="AH25:AH27"/>
-    <mergeCell ref="AH28:AH29"/>
-    <mergeCell ref="AH30:AH31"/>
-    <mergeCell ref="AH32:AH33"/>
-    <mergeCell ref="AH34:AH35"/>
-    <mergeCell ref="AF36:AF37"/>
-    <mergeCell ref="AF38:AF39"/>
-    <mergeCell ref="AF40:AF41"/>
-    <mergeCell ref="AH36:AH37"/>
-    <mergeCell ref="AH38:AH39"/>
-    <mergeCell ref="AH40:AH41"/>
-    <mergeCell ref="AF42:AF43"/>
-    <mergeCell ref="AG25:AG27"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="AG30:AG31"/>
-    <mergeCell ref="AG32:AG33"/>
-    <mergeCell ref="AG34:AG35"/>
-    <mergeCell ref="AG36:AG37"/>
-    <mergeCell ref="AG38:AG39"/>
-    <mergeCell ref="AG40:AG41"/>
-    <mergeCell ref="AG42:AG43"/>
-    <mergeCell ref="AF25:AF27"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AF30:AF31"/>
-    <mergeCell ref="AF32:AF33"/>
-    <mergeCell ref="AF34:AF35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Reset tech and civic cost
</commit_message>
<xml_diff>
--- a/文档/科技市政.xlsx
+++ b/文档/科技市政.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E682FC39-32AC-4BBA-B41B-1BF96EA55AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEB57A2-D435-44DD-9B0D-3083A7622C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="177">
   <si>
     <t>Lvl</t>
   </si>
@@ -543,6 +543,42 @@
   </si>
   <si>
     <t>随机需求提升</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -550,7 +586,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,8 +608,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -583,6 +627,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,7 +663,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -619,6 +681,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AK42" sqref="AK42:AK43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -985,7 +1056,7 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C34" si="0">VLOOKUP(B3,$T$3:$AB$22,9,FALSE)</f>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>161</v>
@@ -998,7 +1069,7 @@
       </c>
       <c r="G3" s="3" t="str">
         <f>_xlfn.CONCAT(D3,A3,E3,C3,F3)</f>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_POTTERY" /&gt;&lt;Set Cost="40"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_POTTERY" /&gt;&lt;Set Cost="30"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H34" si="1">VLOOKUP(B3,$T$3:$U$22,2,FALSE)</f>
@@ -1012,7 +1083,7 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K34" si="2">VLOOKUP(J3,$S$46:$T$75,2,FALSE)</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>164</v>
@@ -1025,7 +1096,7 @@
       </c>
       <c r="O3" s="3" t="str">
         <f>_xlfn.CONCAT(L3,I3,M3,K3,N3)</f>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CODE_OF_LAWS" /&gt;&lt;Set Cost="30"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CODE_OF_LAWS" /&gt;&lt;Set Cost="25"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -1045,11 +1116,14 @@
       <c r="X3">
         <v>20</v>
       </c>
+      <c r="Y3" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="AA3">
         <v>20</v>
       </c>
       <c r="AB3" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AC3" s="1">
         <f t="shared" ref="AC3:AC22" si="3">COUNTIF(B:B,T3)</f>
@@ -1057,7 +1131,7 @@
       </c>
       <c r="AD3" s="1">
         <f>AB3*AC3</f>
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -1069,7 +1143,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>161</v>
@@ -1082,7 +1156,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" ref="G4:G67" si="4">_xlfn.CONCAT(D4,A4,E4,C4,F4)</f>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ANIMAL_HUSBANDRY" /&gt;&lt;Set Cost="40"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ANIMAL_HUSBANDRY" /&gt;&lt;Set Cost="30"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
@@ -1096,7 +1170,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>164</v>
@@ -1109,7 +1183,7 @@
       </c>
       <c r="O4" s="3" t="str">
         <f t="shared" ref="O4:O63" si="5">_xlfn.CONCAT(L4,I4,M4,K4,N4)</f>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CRAFTSMANSHIP" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CRAFTSMANSHIP" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P4">
         <v>2</v>
@@ -1139,6 +1213,9 @@
       <c r="X4" s="1">
         <v>35</v>
       </c>
+      <c r="Y4" s="6" t="s">
+        <v>168</v>
+      </c>
       <c r="Z4">
         <v>10</v>
       </c>
@@ -1148,7 +1225,7 @@
       </c>
       <c r="AB4" s="1">
         <f>AB3+AA4</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AC4" s="1">
         <f t="shared" si="3"/>
@@ -1156,7 +1233,7 @@
       </c>
       <c r="AD4" s="1">
         <f t="shared" ref="AD4:AD22" si="7">AB4*AC4</f>
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -1168,7 +1245,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>161</v>
@@ -1181,7 +1258,7 @@
       </c>
       <c r="G5" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MINING" /&gt;&lt;Set Cost="40"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MINING" /&gt;&lt;Set Cost="30"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -1195,7 +1272,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>164</v>
@@ -1208,7 +1285,7 @@
       </c>
       <c r="O5" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FOREIGN_TRADE" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FOREIGN_TRADE" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P5">
         <v>2</v>
@@ -1238,6 +1315,9 @@
       <c r="X5" s="1">
         <v>55</v>
       </c>
+      <c r="Y5" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="Z5">
         <v>10</v>
       </c>
@@ -1247,7 +1327,7 @@
       </c>
       <c r="AB5" s="1">
         <f>AB4+AA5</f>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="AC5" s="1">
         <f t="shared" si="3"/>
@@ -1255,7 +1335,7 @@
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="7"/>
-        <v>330</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -1267,7 +1347,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>161</v>
@@ -1280,7 +1360,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SAILING" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SAILING" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
@@ -1294,7 +1374,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>164</v>
@@ -1307,7 +1387,7 @@
       </c>
       <c r="O6" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRADITION" /&gt;&lt;Set Cost="105"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRADITION" /&gt;&lt;Set Cost="95"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P6">
         <v>3</v>
@@ -1337,6 +1417,9 @@
       <c r="X6" s="1">
         <v>85</v>
       </c>
+      <c r="Y6" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="Z6">
         <v>10</v>
       </c>
@@ -1346,7 +1429,7 @@
       </c>
       <c r="AB6" s="1">
         <f t="shared" ref="AB6:AB22" si="12">AB5+AA6</f>
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" si="3"/>
@@ -1354,7 +1437,7 @@
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="7"/>
-        <v>640</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -1366,7 +1449,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>161</v>
@@ -1379,7 +1462,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTROLOGY" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTROLOGY" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
@@ -1393,7 +1476,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>164</v>
@@ -1406,7 +1489,7 @@
       </c>
       <c r="O7" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_STATE_WORKFORCE" /&gt;&lt;Set Cost="135"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_STATE_WORKFORCE" /&gt;&lt;Set Cost="125"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P7">
         <v>3</v>
@@ -1436,16 +1519,19 @@
       <c r="X7" s="1">
         <v>105</v>
       </c>
+      <c r="Y7" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="Z7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA7">
         <f t="shared" si="10"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" si="12"/>
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" si="3"/>
@@ -1453,7 +1539,7 @@
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="7"/>
-        <v>920</v>
+        <v>840</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1465,7 +1551,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>161</v>
@@ -1478,7 +1564,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRRIGATION" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRRIGATION" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
@@ -1492,7 +1578,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>164</v>
@@ -1505,7 +1591,7 @@
       </c>
       <c r="O8" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EARLY_EMPIRE" /&gt;&lt;Set Cost="135"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EARLY_EMPIRE" /&gt;&lt;Set Cost="125"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P8">
         <v>3</v>
@@ -1535,16 +1621,19 @@
       <c r="X8" s="1">
         <v>175</v>
       </c>
+      <c r="Y8" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="Z8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA8">
         <f t="shared" si="10"/>
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="AB8" s="1">
         <f t="shared" si="12"/>
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="AC8" s="1">
         <f t="shared" si="3"/>
@@ -1552,7 +1641,7 @@
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="7"/>
-        <v>1280</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -1564,7 +1653,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>161</v>
@@ -1577,7 +1666,7 @@
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ARCHERY" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ARCHERY" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
@@ -1591,7 +1680,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>164</v>
@@ -1604,7 +1693,7 @@
       </c>
       <c r="O9" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MYSTICISM" /&gt;&lt;Set Cost="105"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MYSTICISM" /&gt;&lt;Set Cost="95"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P9">
         <v>3</v>
@@ -1634,16 +1723,19 @@
       <c r="X9" s="1">
         <v>275</v>
       </c>
+      <c r="Y9" s="6" t="s">
+        <v>170</v>
+      </c>
       <c r="Z9">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="AA9">
         <f t="shared" si="10"/>
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="AB9" s="1">
         <f t="shared" si="12"/>
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="AC9" s="1">
         <f t="shared" si="3"/>
@@ -1651,7 +1743,7 @@
       </c>
       <c r="AD9" s="1">
         <f t="shared" si="7"/>
-        <v>1720</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -1663,7 +1755,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>161</v>
@@ -1676,7 +1768,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_WRITING" /&gt;&lt;Set Cost="70"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_WRITING" /&gt;&lt;Set Cost="60"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
@@ -1690,7 +1782,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>164</v>
@@ -1703,7 +1795,7 @@
       </c>
       <c r="O10" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GAMES_RECREATION" /&gt;&lt;Set Cost="190"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GAMES_RECREATION" /&gt;&lt;Set Cost="180"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P10">
         <v>4</v>
@@ -1733,16 +1825,19 @@
       <c r="X10" s="1">
         <v>375</v>
       </c>
+      <c r="Y10" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="Z10">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="AA10">
         <f t="shared" si="10"/>
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="AB10" s="1">
         <f t="shared" si="12"/>
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="AC10" s="1">
         <f t="shared" si="3"/>
@@ -1750,7 +1845,7 @@
       </c>
       <c r="AD10" s="1">
         <f t="shared" si="7"/>
-        <v>2900</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -1762,7 +1857,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>161</v>
@@ -1775,7 +1870,7 @@
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASONRY" /&gt;&lt;Set Cost="110"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASONRY" /&gt;&lt;Set Cost="100"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
@@ -1789,7 +1884,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>164</v>
@@ -1802,7 +1897,7 @@
       </c>
       <c r="O11" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_POLITICAL_PHILOSOPHY" /&gt;&lt;Set Cost="190"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_POLITICAL_PHILOSOPHY" /&gt;&lt;Set Cost="180"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P11">
         <v>4</v>
@@ -1832,16 +1927,19 @@
       <c r="X11" s="1">
         <v>485</v>
       </c>
+      <c r="Y11" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="Z11">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="AA11">
         <f t="shared" si="10"/>
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="AB11" s="1">
         <f t="shared" si="12"/>
-        <v>770</v>
+        <v>700</v>
       </c>
       <c r="AC11" s="1">
         <f t="shared" si="3"/>
@@ -1849,7 +1947,7 @@
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="7"/>
-        <v>3080</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -1861,7 +1959,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>161</v>
@@ -1874,7 +1972,7 @@
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BRONZE_WORKING" /&gt;&lt;Set Cost="110"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BRONZE_WORKING" /&gt;&lt;Set Cost="100"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
@@ -1888,7 +1986,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>164</v>
@@ -1901,7 +1999,7 @@
       </c>
       <c r="O12" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DRAMA_POETRY" /&gt;&lt;Set Cost="190"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DRAMA_POETRY" /&gt;&lt;Set Cost="180"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P12">
         <v>4</v>
@@ -1931,16 +2029,19 @@
       <c r="X12" s="1">
         <v>780</v>
       </c>
+      <c r="Y12" s="6" t="s">
+        <v>172</v>
+      </c>
       <c r="Z12">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="AA12">
         <f t="shared" si="10"/>
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="AB12" s="1">
         <f t="shared" si="12"/>
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="AC12" s="1">
         <f t="shared" si="3"/>
@@ -1948,7 +2049,7 @@
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="7"/>
-        <v>4000</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -1960,7 +2061,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>161</v>
@@ -1973,7 +2074,7 @@
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_THE_WHEEL" /&gt;&lt;Set Cost="110"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_THE_WHEEL" /&gt;&lt;Set Cost="100"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
@@ -1987,7 +2088,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>164</v>
@@ -2000,7 +2101,7 @@
       </c>
       <c r="O13" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRAINING" /&gt;&lt;Set Cost="250"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MILITARY_TRAINING" /&gt;&lt;Set Cost="240"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P13">
         <v>5</v>
@@ -2030,16 +2131,19 @@
       <c r="X13" s="1">
         <v>1150</v>
       </c>
+      <c r="Y13" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="Z13">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="AA13">
         <f t="shared" si="10"/>
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="AB13" s="1">
         <f t="shared" si="12"/>
-        <v>1310</v>
+        <v>1240</v>
       </c>
       <c r="AC13" s="1">
         <f t="shared" si="3"/>
@@ -2047,7 +2151,7 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="7"/>
-        <v>5240</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -2059,7 +2163,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>161</v>
@@ -2072,7 +2176,7 @@
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CELESTIAL_NAVIGATION" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CELESTIAL_NAVIGATION" /&gt;&lt;Set Cost="150"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
@@ -2086,7 +2190,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>164</v>
@@ -2099,7 +2203,7 @@
       </c>
       <c r="O14" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DEFENSIVE_TACTICS" /&gt;&lt;Set Cost="310"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DEFENSIVE_TACTICS" /&gt;&lt;Set Cost="300"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P14">
         <v>5</v>
@@ -2129,16 +2233,19 @@
       <c r="X14" s="1">
         <v>1600</v>
       </c>
+      <c r="Y14" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="Z14">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="AA14">
         <f t="shared" si="10"/>
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="AB14" s="1">
         <f t="shared" si="12"/>
-        <v>1700</v>
+        <v>1540</v>
       </c>
       <c r="AC14" s="1">
         <f t="shared" si="3"/>
@@ -2146,7 +2253,7 @@
       </c>
       <c r="AD14" s="1">
         <f t="shared" si="7"/>
-        <v>6800</v>
+        <v>6160</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -2158,7 +2265,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>161</v>
@@ -2171,7 +2278,7 @@
       </c>
       <c r="G15" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CURRENCY" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CURRENCY" /&gt;&lt;Set Cost="150"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
@@ -2185,7 +2292,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>164</v>
@@ -2198,7 +2305,7 @@
       </c>
       <c r="O15" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RECORDED_HISTORY" /&gt;&lt;Set Cost="310"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RECORDED_HISTORY" /&gt;&lt;Set Cost="300"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P15">
         <v>5</v>
@@ -2228,16 +2335,19 @@
       <c r="X15" s="1">
         <v>2350</v>
       </c>
+      <c r="Y15" s="6" t="s">
+        <v>173</v>
+      </c>
       <c r="Z15">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="AA15">
         <f t="shared" si="10"/>
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="AB15" s="1">
         <f t="shared" si="12"/>
-        <v>2170</v>
+        <v>1990</v>
       </c>
       <c r="AC15" s="1">
         <f t="shared" si="3"/>
@@ -2245,7 +2355,7 @@
       </c>
       <c r="AD15" s="1">
         <f t="shared" si="7"/>
-        <v>8680</v>
+        <v>7960</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2257,7 +2367,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>161</v>
@@ -2270,7 +2380,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_HORSEBACK_RIDING" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_HORSEBACK_RIDING" /&gt;&lt;Set Cost="150"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
@@ -2284,7 +2394,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>164</v>
@@ -2297,7 +2407,7 @@
       </c>
       <c r="O16" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THEOLOGY" /&gt;&lt;Set Cost="250"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THEOLOGY" /&gt;&lt;Set Cost="240"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P16">
         <v>5</v>
@@ -2327,16 +2437,19 @@
       <c r="X16" s="1">
         <v>3100</v>
       </c>
+      <c r="Y16" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="Z16">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="AA16">
         <f t="shared" si="10"/>
-        <v>570</v>
+        <v>470</v>
       </c>
       <c r="AB16" s="1">
         <f t="shared" si="12"/>
-        <v>2740</v>
+        <v>2460</v>
       </c>
       <c r="AC16" s="1">
         <f t="shared" si="3"/>
@@ -2344,7 +2457,7 @@
       </c>
       <c r="AD16" s="1">
         <f t="shared" si="7"/>
-        <v>13700</v>
+        <v>12300</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
@@ -2356,7 +2469,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>161</v>
@@ -2369,7 +2482,7 @@
       </c>
       <c r="G17" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRON_WORKING" /&gt;&lt;Set Cost="160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_IRON_WORKING" /&gt;&lt;Set Cost="150"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
@@ -2383,7 +2496,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>164</v>
@@ -2396,7 +2509,7 @@
       </c>
       <c r="O17" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NAVAL_TRADITION" /&gt;&lt;Set Cost="355"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NAVAL_TRADITION" /&gt;&lt;Set Cost="335"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P17">
         <v>6</v>
@@ -2426,16 +2539,19 @@
       <c r="X17" s="1">
         <v>4100</v>
       </c>
+      <c r="Y17" s="7" t="s">
+        <v>174</v>
+      </c>
       <c r="Z17">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="AA17">
         <f t="shared" si="10"/>
-        <v>670</v>
+        <v>490</v>
       </c>
       <c r="AB17" s="1">
         <f t="shared" si="12"/>
-        <v>3410</v>
+        <v>2950</v>
       </c>
       <c r="AC17" s="1">
         <f t="shared" si="3"/>
@@ -2443,7 +2559,7 @@
       </c>
       <c r="AD17" s="1">
         <f t="shared" si="7"/>
-        <v>10230</v>
+        <v>8850</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
@@ -2455,7 +2571,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>161</v>
@@ -2468,7 +2584,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SHIPBUILDING" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SHIPBUILDING" /&gt;&lt;Set Cost="210"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
@@ -2482,7 +2598,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>164</v>
@@ -2495,7 +2611,7 @@
       </c>
       <c r="O18" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FEUDALISM" /&gt;&lt;Set Cost="445"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FEUDALISM" /&gt;&lt;Set Cost="425"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P18">
         <v>6</v>
@@ -2525,16 +2641,19 @@
       <c r="X18" s="1">
         <v>5100</v>
       </c>
+      <c r="Y18" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="Z18">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="AA18">
         <f t="shared" si="10"/>
-        <v>790</v>
+        <v>510</v>
       </c>
       <c r="AB18" s="1">
         <f t="shared" si="12"/>
-        <v>4200</v>
+        <v>3460</v>
       </c>
       <c r="AC18" s="1">
         <f t="shared" si="3"/>
@@ -2542,7 +2661,7 @@
       </c>
       <c r="AD18" s="1">
         <f t="shared" si="7"/>
-        <v>25200</v>
+        <v>20760</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
@@ -2554,7 +2673,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>161</v>
@@ -2567,7 +2686,7 @@
       </c>
       <c r="G19" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MATHEMATICS" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MATHEMATICS" /&gt;&lt;Set Cost="210"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
@@ -2581,7 +2700,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>164</v>
@@ -2594,7 +2713,7 @@
       </c>
       <c r="O19" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_SERVICE" /&gt;&lt;Set Cost="445"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_SERVICE" /&gt;&lt;Set Cost="425"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P19">
         <v>6</v>
@@ -2624,16 +2743,19 @@
       <c r="X19" s="1">
         <v>6400</v>
       </c>
+      <c r="Y19" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="Z19">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="AA19">
         <f t="shared" si="10"/>
-        <v>910</v>
+        <v>530</v>
       </c>
       <c r="AB19" s="1">
         <f t="shared" si="12"/>
-        <v>5110</v>
+        <v>3990</v>
       </c>
       <c r="AC19" s="1">
         <f t="shared" si="3"/>
@@ -2641,7 +2763,7 @@
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="7"/>
-        <v>15330</v>
+        <v>11970</v>
       </c>
       <c r="AE19" s="3" t="s">
         <v>167</v>
@@ -2656,7 +2778,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>161</v>
@@ -2669,7 +2791,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CONSTRUCTION" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CONSTRUCTION" /&gt;&lt;Set Cost="210"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
@@ -2683,7 +2805,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
-        <v>505</v>
+        <v>465</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>164</v>
@@ -2696,7 +2818,7 @@
       </c>
       <c r="O20" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCENARIES" /&gt;&lt;Set Cost="505"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCENARIES" /&gt;&lt;Set Cost="465"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P20">
         <v>7</v>
@@ -2726,16 +2848,19 @@
       <c r="X20" s="1">
         <v>7700</v>
       </c>
+      <c r="Y20" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="Z20">
-        <v>140</v>
+        <v>20</v>
       </c>
       <c r="AA20">
         <f t="shared" si="10"/>
-        <v>1050</v>
+        <v>550</v>
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="12"/>
-        <v>6160</v>
+        <v>4540</v>
       </c>
       <c r="AC20" s="1">
         <f t="shared" si="3"/>
@@ -2743,11 +2868,11 @@
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="7"/>
-        <v>36960</v>
+        <v>27240</v>
       </c>
       <c r="AE20">
         <f>AB20+0.5*AA21</f>
-        <v>6755</v>
+        <v>4825</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
@@ -2759,7 +2884,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>161</v>
@@ -2772,7 +2897,7 @@
       </c>
       <c r="G21" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ENGINEERING" /&gt;&lt;Set Cost="230"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ENGINEERING" /&gt;&lt;Set Cost="210"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
@@ -2786,7 +2911,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="2"/>
-        <v>595</v>
+        <v>555</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>164</v>
@@ -2799,7 +2924,7 @@
       </c>
       <c r="O21" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MEDIEVAL_FAIRES" /&gt;&lt;Set Cost="595"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MEDIEVAL_FAIRES" /&gt;&lt;Set Cost="555"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P21">
         <v>7</v>
@@ -2829,16 +2954,19 @@
       <c r="X21" s="1">
         <v>8800</v>
       </c>
+      <c r="Y21" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="Z21">
-        <v>140</v>
+        <v>20</v>
       </c>
       <c r="AA21">
         <f t="shared" si="10"/>
-        <v>1190</v>
+        <v>570</v>
       </c>
       <c r="AB21" s="1">
         <f t="shared" si="12"/>
-        <v>7350</v>
+        <v>5110</v>
       </c>
       <c r="AC21" s="1">
         <f t="shared" si="3"/>
@@ -2846,7 +2974,7 @@
       </c>
       <c r="AD21" s="1">
         <f t="shared" si="7"/>
-        <v>7350</v>
+        <v>5110</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
@@ -2858,7 +2986,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>161</v>
@@ -2871,7 +2999,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_TACTICS" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_TACTICS" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
@@ -2885,7 +3013,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
-        <v>595</v>
+        <v>555</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>164</v>
@@ -2898,7 +3026,7 @@
       </c>
       <c r="O22" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GUILDS" /&gt;&lt;Set Cost="595"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GUILDS" /&gt;&lt;Set Cost="555"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P22">
         <v>7</v>
@@ -2928,16 +3056,19 @@
       <c r="X22" s="1">
         <v>9500</v>
       </c>
+      <c r="Y22" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="Z22">
-        <v>-540</v>
+        <v>-280</v>
       </c>
       <c r="AA22">
         <f t="shared" si="10"/>
-        <v>650</v>
+        <v>290</v>
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="12"/>
-        <v>8000</v>
+        <v>5400</v>
       </c>
       <c r="AC22" s="1">
         <f t="shared" si="3"/>
@@ -2945,7 +3076,7 @@
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="7"/>
-        <v>8000</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
@@ -2957,7 +3088,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>161</v>
@@ -2970,7 +3101,7 @@
       </c>
       <c r="G23" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_APPRENTICESHIP" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_APPRENTICESHIP" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
@@ -2984,7 +3115,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="2"/>
-        <v>505</v>
+        <v>465</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>164</v>
@@ -2997,7 +3128,7 @@
       </c>
       <c r="O23" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIVINE_RIGHT" /&gt;&lt;Set Cost="505"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIVINE_RIGHT" /&gt;&lt;Set Cost="465"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P23">
         <v>7</v>
@@ -3018,7 +3149,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>161</v>
@@ -3031,7 +3162,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MACHINERY" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MACHINERY" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
@@ -3045,7 +3176,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
-        <v>690</v>
+        <v>630</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>164</v>
@@ -3058,7 +3189,7 @@
       </c>
       <c r="O24" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXPLORATION" /&gt;&lt;Set Cost="690"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXPLORATION" /&gt;&lt;Set Cost="630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P24">
         <v>8</v>
@@ -3130,7 +3261,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>161</v>
@@ -3143,7 +3274,7 @@
       </c>
       <c r="G25" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_EDUCATION" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_EDUCATION" /&gt;&lt;Set Cost="400"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
@@ -3157,7 +3288,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
-        <v>810</v>
+        <v>750</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>164</v>
@@ -3170,7 +3301,7 @@
       </c>
       <c r="O25" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_HUMANISM" /&gt;&lt;Set Cost="810"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_HUMANISM" /&gt;&lt;Set Cost="750"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P25">
         <v>8</v>
@@ -3200,52 +3331,54 @@
         <v>0</v>
       </c>
       <c r="Y25">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Z25">
         <f>0+Y25</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AA25">
         <v>0</v>
       </c>
       <c r="AB25">
         <f t="shared" ref="AB25:AB28" si="14">Z25-0.5*AA25</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AC25">
         <f t="shared" ref="AC25:AC28" si="15">Z25+0.5*AA25</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AD25">
         <f t="shared" ref="AD25:AD44" si="16">Z25*W25</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AE25">
         <f t="shared" ref="AE25:AE44" si="17">AD3</f>
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="AF25" s="4">
         <f>AD25+AD26+AD27</f>
-        <v>650</v>
+        <v>585</v>
       </c>
       <c r="AG25" s="4">
         <f>AE25+AE26+AE27</f>
-        <v>800</v>
+        <v>690</v>
       </c>
       <c r="AH25" s="4">
         <f>AF25</f>
-        <v>650</v>
+        <v>585</v>
       </c>
       <c r="AI25" s="4">
         <f>AG25</f>
-        <v>800</v>
+        <v>690</v>
       </c>
       <c r="AJ25" s="4">
         <f>AH25-AI25</f>
-        <v>-150</v>
-      </c>
-      <c r="AK25" s="4"/>
+        <v>-105</v>
+      </c>
+      <c r="AK25" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="AL25" s="4"/>
       <c r="AM25" s="4"/>
     </row>
@@ -3258,7 +3391,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>161</v>
@@ -3271,7 +3404,7 @@
       </c>
       <c r="G26" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STIRRUPS" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STIRRUPS" /&gt;&lt;Set Cost="400"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
@@ -3285,7 +3418,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="2"/>
-        <v>810</v>
+        <v>750</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>164</v>
@@ -3298,7 +3431,7 @@
       </c>
       <c r="O26" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIPLOMATIC_SERVICE" /&gt;&lt;Set Cost="810"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIPLOMATIC_SERVICE" /&gt;&lt;Set Cost="750"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P26">
         <v>8</v>
@@ -3329,37 +3462,39 @@
       </c>
       <c r="Y26">
         <f>Y25+X26</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="Z26">
         <f>Z25+Y26</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AA26">
         <v>0</v>
       </c>
       <c r="AB26">
         <f t="shared" si="14"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AC26">
         <f t="shared" si="15"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AD26">
         <f t="shared" si="16"/>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="AE26">
         <f t="shared" si="17"/>
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4"/>
       <c r="AI26" s="4"/>
       <c r="AJ26" s="4"/>
-      <c r="AK26" s="4"/>
+      <c r="AK26" s="6" t="s">
+        <v>168</v>
+      </c>
       <c r="AL26" s="4"/>
       <c r="AM26" s="4"/>
     </row>
@@ -3372,7 +3507,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>161</v>
@@ -3385,7 +3520,7 @@
       </c>
       <c r="G27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_ENGINEERING" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_ENGINEERING" /&gt;&lt;Set Cost="400"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
@@ -3399,7 +3534,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="2"/>
-        <v>690</v>
+        <v>630</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>164</v>
@@ -3412,7 +3547,7 @@
       </c>
       <c r="O27" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_REFORMED_CHURCH" /&gt;&lt;Set Cost="690"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_REFORMED_CHURCH" /&gt;&lt;Set Cost="630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P27">
         <v>8</v>
@@ -3439,7 +3574,7 @@
         <v>4</v>
       </c>
       <c r="X27">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Y27">
         <f t="shared" ref="Y27:Y43" si="19">Y26+X27</f>
@@ -3447,33 +3582,35 @@
       </c>
       <c r="Z27">
         <f t="shared" ref="Z27:Z43" si="20">Z26+Y27</f>
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AA27">
         <v>30</v>
       </c>
       <c r="AB27">
         <f t="shared" si="14"/>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="AC27">
         <f t="shared" si="15"/>
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="AD27">
         <f t="shared" si="16"/>
-        <v>480</v>
+        <v>440</v>
       </c>
       <c r="AE27">
         <f t="shared" si="17"/>
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
       <c r="AH27" s="4"/>
       <c r="AI27" s="4"/>
       <c r="AJ27" s="4"/>
-      <c r="AK27" s="4"/>
+      <c r="AK27" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="AL27" s="4"/>
       <c r="AM27" s="4"/>
     </row>
@@ -3486,7 +3623,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>161</v>
@@ -3499,7 +3636,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CASTLES" /&gt;&lt;Set Cost="430"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CASTLES" /&gt;&lt;Set Cost="400"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
@@ -3513,7 +3650,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>164</v>
@@ -3526,7 +3663,7 @@
       </c>
       <c r="O28" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCANTILISM" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MERCANTILISM" /&gt;&lt;Set Cost="900"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P28">
         <v>9</v>
@@ -3561,48 +3698,50 @@
       </c>
       <c r="Z28">
         <f t="shared" si="20"/>
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="AA28">
         <v>0</v>
       </c>
       <c r="AB28">
         <f t="shared" si="14"/>
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="AC28">
         <f t="shared" si="15"/>
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="AD28">
         <f t="shared" si="16"/>
-        <v>570</v>
+        <v>540</v>
       </c>
       <c r="AE28">
         <f t="shared" si="17"/>
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="AF28" s="4">
         <f>AD28+AD29</f>
-        <v>1410</v>
+        <v>1350</v>
       </c>
       <c r="AG28" s="4">
         <f>AE28+AE29</f>
-        <v>1560</v>
+        <v>1440</v>
       </c>
       <c r="AH28" s="4">
         <f>AH25+AF28</f>
-        <v>2060</v>
+        <v>1935</v>
       </c>
       <c r="AI28" s="4">
         <f>AI25+AG28</f>
-        <v>2360</v>
+        <v>2130</v>
       </c>
       <c r="AJ28" s="4">
         <f>AH28-AI28</f>
-        <v>-300</v>
-      </c>
-      <c r="AK28" s="4"/>
+        <v>-195</v>
+      </c>
+      <c r="AK28" s="8" t="s">
+        <v>169</v>
+      </c>
       <c r="AL28" s="4"/>
       <c r="AM28" s="4"/>
     </row>
@@ -3615,7 +3754,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>161</v>
@@ -3628,7 +3767,7 @@
       </c>
       <c r="G29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CARTOGRAPHY" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CARTOGRAPHY" /&gt;&lt;Set Cost="540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
@@ -3642,7 +3781,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>164</v>
@@ -3655,7 +3794,7 @@
       </c>
       <c r="O29" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THE_ENLIGHTENMENT" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_THE_ENLIGHTENMENT" /&gt;&lt;Set Cost="900"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P29">
         <v>9</v>
@@ -3689,33 +3828,35 @@
       </c>
       <c r="Z29">
         <f t="shared" si="20"/>
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="AA29">
         <v>60</v>
       </c>
       <c r="AB29">
         <f t="shared" ref="AB29" si="21">Z29-0.5*AA29</f>
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="AC29">
         <f t="shared" ref="AC29" si="22">Z29+0.5*AA29</f>
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="AD29">
         <f t="shared" si="16"/>
-        <v>840</v>
+        <v>810</v>
       </c>
       <c r="AE29">
         <f t="shared" si="17"/>
-        <v>920</v>
+        <v>840</v>
       </c>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
       <c r="AH29" s="4"/>
       <c r="AI29" s="4"/>
       <c r="AJ29" s="4"/>
-      <c r="AK29" s="4"/>
+      <c r="AK29" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="AL29" s="4"/>
       <c r="AM29" s="4"/>
     </row>
@@ -3728,7 +3869,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>161</v>
@@ -3741,7 +3882,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASS_PRODUCTION" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MASS_PRODUCTION" /&gt;&lt;Set Cost="540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
@@ -3755,7 +3896,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
-        <v>1245</v>
+        <v>1135</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>164</v>
@@ -3768,7 +3909,7 @@
       </c>
       <c r="O30" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLONIALISM" /&gt;&lt;Set Cost="1245"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLONIALISM" /&gt;&lt;Set Cost="1135"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P30">
         <v>10</v>
@@ -3794,56 +3935,58 @@
         <v>3</v>
       </c>
       <c r="X30">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Y30">
         <f t="shared" si="19"/>
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="Z30">
         <f t="shared" si="20"/>
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="AA30">
         <v>90</v>
       </c>
       <c r="AB30">
         <f t="shared" ref="AB30:AB44" si="23">Z30-0.5*AA30</f>
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="AC30">
         <f t="shared" ref="AC30:AC44" si="24">Z30+0.5*AA30</f>
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="AD30">
         <f t="shared" si="16"/>
-        <v>1200</v>
+        <v>1140</v>
       </c>
       <c r="AE30">
         <f t="shared" si="17"/>
-        <v>1280</v>
+        <v>1120</v>
       </c>
       <c r="AF30" s="4">
         <f>AD30+AD31</f>
-        <v>2850</v>
+        <v>2670</v>
       </c>
       <c r="AG30" s="4">
         <f>AE30+AE31</f>
-        <v>3000</v>
+        <v>2720</v>
       </c>
       <c r="AH30" s="4">
         <f>AH28+AF30</f>
-        <v>4910</v>
+        <v>4605</v>
       </c>
       <c r="AI30" s="4">
         <f>AI28+AG30</f>
-        <v>5360</v>
+        <v>4850</v>
       </c>
       <c r="AJ30" s="4">
         <f>AH30-AI30</f>
-        <v>-450</v>
-      </c>
-      <c r="AK30" s="4"/>
+        <v>-245</v>
+      </c>
+      <c r="AK30" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="AL30" s="4"/>
       <c r="AM30" s="4"/>
     </row>
@@ -3856,7 +3999,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>161</v>
@@ -3869,7 +4012,7 @@
       </c>
       <c r="G31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BANKING" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BANKING" /&gt;&lt;Set Cost="540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
@@ -3883,7 +4026,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="2"/>
-        <v>1395</v>
+        <v>1285</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>164</v>
@@ -3896,7 +4039,7 @@
       </c>
       <c r="O31" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_ENGINEERING" /&gt;&lt;Set Cost="1395"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CIVIL_ENGINEERING" /&gt;&lt;Set Cost="1285"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P31">
         <v>10</v>
@@ -3922,41 +4065,43 @@
         <v>3</v>
       </c>
       <c r="X31">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Y31">
         <f t="shared" si="19"/>
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="Z31">
         <f t="shared" si="20"/>
-        <v>550</v>
+        <v>510</v>
       </c>
       <c r="AA31">
         <v>90</v>
       </c>
       <c r="AB31">
         <f t="shared" si="23"/>
-        <v>505</v>
+        <v>465</v>
       </c>
       <c r="AC31">
         <f t="shared" si="24"/>
-        <v>595</v>
+        <v>555</v>
       </c>
       <c r="AD31">
         <f t="shared" si="16"/>
-        <v>1650</v>
+        <v>1530</v>
       </c>
       <c r="AE31">
         <f t="shared" si="17"/>
-        <v>1720</v>
+        <v>1600</v>
       </c>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
       <c r="AH31" s="4"/>
       <c r="AI31" s="4"/>
       <c r="AJ31" s="4"/>
-      <c r="AK31" s="4"/>
+      <c r="AK31" s="6" t="s">
+        <v>170</v>
+      </c>
       <c r="AL31" s="4"/>
       <c r="AM31" s="4"/>
     </row>
@@ -3969,7 +4114,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>161</v>
@@ -3982,7 +4127,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUNPOWDER" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUNPOWDER" /&gt;&lt;Set Cost="540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
@@ -3996,7 +4141,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="2"/>
-        <v>1395</v>
+        <v>1285</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>164</v>
@@ -4009,7 +4154,7 @@
       </c>
       <c r="O32" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATIONALISM" /&gt;&lt;Set Cost="1395"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATIONALISM" /&gt;&lt;Set Cost="1285"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P32">
         <v>10</v>
@@ -4039,52 +4184,54 @@
       </c>
       <c r="Y32">
         <f t="shared" si="19"/>
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="Z32">
         <f t="shared" si="20"/>
-        <v>750</v>
+        <v>690</v>
       </c>
       <c r="AA32">
         <v>120</v>
       </c>
       <c r="AB32">
         <f t="shared" si="23"/>
-        <v>690</v>
+        <v>630</v>
       </c>
       <c r="AC32">
         <f t="shared" si="24"/>
-        <v>810</v>
+        <v>750</v>
       </c>
       <c r="AD32">
         <f t="shared" si="16"/>
-        <v>2250</v>
+        <v>2070</v>
       </c>
       <c r="AE32">
         <f t="shared" si="17"/>
-        <v>2900</v>
+        <v>2700</v>
       </c>
       <c r="AF32" s="4">
         <f>AD32+AD33</f>
-        <v>4250</v>
+        <v>3870</v>
       </c>
       <c r="AG32" s="4">
         <f>AE32+AE33</f>
-        <v>5980</v>
+        <v>5500</v>
       </c>
       <c r="AH32" s="4">
         <f>AH30+AF32</f>
-        <v>9160</v>
+        <v>8475</v>
       </c>
       <c r="AI32" s="4">
         <f>AI30+AG32</f>
-        <v>11340</v>
+        <v>10350</v>
       </c>
       <c r="AJ32" s="4">
         <f>AH32-AI32</f>
-        <v>-2180</v>
-      </c>
-      <c r="AK32" s="4"/>
+        <v>-1875</v>
+      </c>
+      <c r="AK32" s="8" t="s">
+        <v>171</v>
+      </c>
       <c r="AL32" s="4"/>
       <c r="AM32" s="4"/>
     </row>
@@ -4097,7 +4244,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>161</v>
@@ -4110,7 +4257,7 @@
       </c>
       <c r="G33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PRINTING" /&gt;&lt;Set Cost="580"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PRINTING" /&gt;&lt;Set Cost="540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
@@ -4124,7 +4271,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="2"/>
-        <v>1245</v>
+        <v>1135</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>164</v>
@@ -4137,7 +4284,7 @@
       </c>
       <c r="O33" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_OPERA_BALLET" /&gt;&lt;Set Cost="1245"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_OPERA_BALLET" /&gt;&lt;Set Cost="1135"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P33">
         <v>10</v>
@@ -4164,41 +4311,43 @@
         <v>2</v>
       </c>
       <c r="X33">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="Y33">
         <f t="shared" si="19"/>
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="Z33">
         <f t="shared" si="20"/>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="AA33">
         <v>0</v>
       </c>
       <c r="AB33">
         <f t="shared" si="23"/>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="AC33">
         <f t="shared" si="24"/>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="AD33">
         <f t="shared" si="16"/>
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="AE33">
         <f t="shared" si="17"/>
-        <v>3080</v>
+        <v>2800</v>
       </c>
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
       <c r="AH33" s="4"/>
       <c r="AI33" s="4"/>
       <c r="AJ33" s="4"/>
-      <c r="AK33" s="4"/>
+      <c r="AK33" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="AL33" s="4"/>
       <c r="AM33" s="4"/>
     </row>
@@ -4211,7 +4360,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>770</v>
+        <v>700</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>161</v>
@@ -4224,7 +4373,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SQUARE_RIGGING" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SQUARE_RIGGING" /&gt;&lt;Set Cost="700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
@@ -4238,7 +4387,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="2"/>
-        <v>1635</v>
+        <v>1475</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>164</v>
@@ -4251,7 +4400,7 @@
       </c>
       <c r="O34" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATURAL_HISTORY" /&gt;&lt;Set Cost="1635"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NATURAL_HISTORY" /&gt;&lt;Set Cost="1475"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P34">
         <v>11</v>
@@ -4278,56 +4427,58 @@
         <v>4</v>
       </c>
       <c r="X34">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="Y34">
         <f t="shared" si="19"/>
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="Z34">
         <f t="shared" si="20"/>
-        <v>1320</v>
+        <v>1210</v>
       </c>
       <c r="AA34">
         <v>150</v>
       </c>
       <c r="AB34">
         <f t="shared" si="23"/>
-        <v>1245</v>
+        <v>1135</v>
       </c>
       <c r="AC34">
         <f t="shared" si="24"/>
-        <v>1395</v>
+        <v>1285</v>
       </c>
       <c r="AD34">
         <f t="shared" si="16"/>
-        <v>5280</v>
+        <v>4840</v>
       </c>
       <c r="AE34">
         <f t="shared" si="17"/>
-        <v>4000</v>
+        <v>3840</v>
       </c>
       <c r="AF34" s="4">
         <f>AD34+AD35</f>
-        <v>10410</v>
+        <v>9490</v>
       </c>
       <c r="AG34" s="4">
         <f>AE34+AE35</f>
-        <v>9240</v>
+        <v>8800</v>
       </c>
       <c r="AH34" s="4">
         <f>AH32+AF34</f>
-        <v>19570</v>
+        <v>17965</v>
       </c>
       <c r="AI34" s="4">
         <f>AI32+AG34</f>
-        <v>20580</v>
+        <v>19150</v>
       </c>
       <c r="AJ34" s="4">
         <f>AH34-AI34</f>
-        <v>-1010</v>
-      </c>
-      <c r="AK34" s="4"/>
+        <v>-1185</v>
+      </c>
+      <c r="AK34" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="AL34" s="4"/>
       <c r="AM34" s="4"/>
     </row>
@@ -4340,7 +4491,7 @@
       </c>
       <c r="C35">
         <f t="shared" ref="C35:C66" si="25">VLOOKUP(B35,$T$3:$AB$22,9,FALSE)</f>
-        <v>770</v>
+        <v>700</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>161</v>
@@ -4353,7 +4504,7 @@
       </c>
       <c r="G35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTRONOMY" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ASTRONOMY" /&gt;&lt;Set Cost="700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H35">
         <f t="shared" ref="H35:H66" si="26">VLOOKUP(B35,$T$3:$U$22,2,FALSE)</f>
@@ -4367,7 +4518,7 @@
       </c>
       <c r="K35">
         <f t="shared" ref="K35:K63" si="27">VLOOKUP(J35,$S$46:$T$75,2,FALSE)</f>
-        <v>1785</v>
+        <v>1625</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>164</v>
@@ -4380,7 +4531,7 @@
       </c>
       <c r="O35" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SCORCHED_EARTH" /&gt;&lt;Set Cost="1785"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SCORCHED_EARTH" /&gt;&lt;Set Cost="1625"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P35">
         <v>11</v>
@@ -4406,41 +4557,43 @@
         <v>3</v>
       </c>
       <c r="X35">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="Y35">
         <f t="shared" si="19"/>
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="Z35">
         <f t="shared" si="20"/>
-        <v>1710</v>
+        <v>1550</v>
       </c>
       <c r="AA35">
         <v>150</v>
       </c>
       <c r="AB35">
         <f t="shared" si="23"/>
-        <v>1635</v>
+        <v>1475</v>
       </c>
       <c r="AC35">
         <f t="shared" si="24"/>
-        <v>1785</v>
+        <v>1625</v>
       </c>
       <c r="AD35">
         <f t="shared" si="16"/>
-        <v>5130</v>
+        <v>4650</v>
       </c>
       <c r="AE35">
         <f t="shared" si="17"/>
-        <v>5240</v>
+        <v>4960</v>
       </c>
       <c r="AF35" s="4"/>
       <c r="AG35" s="4"/>
       <c r="AH35" s="4"/>
       <c r="AI35" s="4"/>
       <c r="AJ35" s="4"/>
-      <c r="AK35" s="4"/>
+      <c r="AK35" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="AL35" s="4"/>
       <c r="AM35" s="4"/>
     </row>
@@ -4453,7 +4606,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="25"/>
-        <v>770</v>
+        <v>700</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>161</v>
@@ -4466,7 +4619,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_METAL_CASTING" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_METAL_CASTING" /&gt;&lt;Set Cost="700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H36">
         <f t="shared" si="26"/>
@@ -4480,7 +4633,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="27"/>
-        <v>1785</v>
+        <v>1625</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>164</v>
@@ -4493,7 +4646,7 @@
       </c>
       <c r="O36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_URBANIZATION" /&gt;&lt;Set Cost="1785"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_URBANIZATION" /&gt;&lt;Set Cost="1625"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P36">
         <v>11</v>
@@ -4519,56 +4672,58 @@
         <v>4</v>
       </c>
       <c r="X36">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="Y36">
         <f t="shared" si="19"/>
-        <v>480</v>
+        <v>370</v>
       </c>
       <c r="Z36">
         <f t="shared" si="20"/>
-        <v>2190</v>
+        <v>1920</v>
       </c>
       <c r="AA36">
         <v>120</v>
       </c>
       <c r="AB36">
         <f t="shared" si="23"/>
-        <v>2130</v>
+        <v>1860</v>
       </c>
       <c r="AC36">
         <f t="shared" si="24"/>
-        <v>2250</v>
+        <v>1980</v>
       </c>
       <c r="AD36">
         <f t="shared" si="16"/>
-        <v>8760</v>
+        <v>7680</v>
       </c>
       <c r="AE36">
         <f t="shared" si="17"/>
-        <v>6800</v>
+        <v>6160</v>
       </c>
       <c r="AF36" s="4">
         <f>AD36+AD37</f>
-        <v>14280</v>
+        <v>12560</v>
       </c>
       <c r="AG36" s="4">
         <f>AE36+AE37</f>
-        <v>15480</v>
+        <v>14120</v>
       </c>
       <c r="AH36" s="4">
         <f t="shared" ref="AH36:AH40" si="28">AH34+AF36</f>
-        <v>33850</v>
+        <v>30525</v>
       </c>
       <c r="AI36" s="4">
         <f t="shared" ref="AI36:AI40" si="29">AI34+AG36</f>
-        <v>36060</v>
+        <v>33270</v>
       </c>
       <c r="AJ36" s="4">
         <f>AH36-AI36</f>
-        <v>-2210</v>
-      </c>
-      <c r="AK36" s="4"/>
+        <v>-2745</v>
+      </c>
+      <c r="AK36" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="AL36" s="4"/>
       <c r="AM36" s="4"/>
     </row>
@@ -4581,7 +4736,7 @@
       </c>
       <c r="C37">
         <f t="shared" si="25"/>
-        <v>770</v>
+        <v>700</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>161</v>
@@ -4594,7 +4749,7 @@
       </c>
       <c r="G37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SIEGE_TACTICS" /&gt;&lt;Set Cost="770"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SIEGE_TACTICS" /&gt;&lt;Set Cost="700"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H37">
         <f t="shared" si="26"/>
@@ -4608,7 +4763,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="27"/>
-        <v>2130</v>
+        <v>1860</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>164</v>
@@ -4621,7 +4776,7 @@
       </c>
       <c r="O37" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CONSERVATION" /&gt;&lt;Set Cost="2130"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CONSERVATION" /&gt;&lt;Set Cost="1860"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P37">
         <v>12</v>
@@ -4647,41 +4802,43 @@
         <v>2</v>
       </c>
       <c r="X37">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="Y37">
         <f t="shared" si="19"/>
-        <v>570</v>
+        <v>520</v>
       </c>
       <c r="Z37">
         <f t="shared" si="20"/>
-        <v>2760</v>
+        <v>2440</v>
       </c>
       <c r="AA37">
         <v>120</v>
       </c>
       <c r="AB37">
         <f t="shared" si="23"/>
-        <v>2700</v>
+        <v>2380</v>
       </c>
       <c r="AC37">
         <f t="shared" si="24"/>
-        <v>2820</v>
+        <v>2500</v>
       </c>
       <c r="AD37">
         <f t="shared" si="16"/>
-        <v>5520</v>
+        <v>4880</v>
       </c>
       <c r="AE37">
         <f t="shared" si="17"/>
-        <v>8680</v>
+        <v>7960</v>
       </c>
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
       <c r="AH37" s="4"/>
       <c r="AI37" s="4"/>
       <c r="AJ37" s="4"/>
-      <c r="AK37" s="4"/>
+      <c r="AK37" s="8" t="s">
+        <v>173</v>
+      </c>
       <c r="AL37" s="4"/>
       <c r="AM37" s="4"/>
     </row>
@@ -4694,7 +4851,7 @@
       </c>
       <c r="C38">
         <f t="shared" si="25"/>
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>161</v>
@@ -4707,7 +4864,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_INDUSTRIALIZATION" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_INDUSTRIALIZATION" /&gt;&lt;Set Cost="960"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H38">
         <f t="shared" si="26"/>
@@ -4721,7 +4878,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="27"/>
-        <v>2250</v>
+        <v>1980</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>164</v>
@@ -4734,7 +4891,7 @@
       </c>
       <c r="O38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CAPITALISM" /&gt;&lt;Set Cost="2250"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CAPITALISM" /&gt;&lt;Set Cost="1980"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P38">
         <v>12</v>
@@ -4760,56 +4917,58 @@
         <v>3</v>
       </c>
       <c r="X38">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="Y38">
         <f t="shared" si="19"/>
-        <v>720</v>
+        <v>570</v>
       </c>
       <c r="Z38">
         <f t="shared" si="20"/>
-        <v>3480</v>
+        <v>3010</v>
       </c>
       <c r="AA38">
         <v>160</v>
       </c>
       <c r="AB38">
         <f t="shared" si="23"/>
-        <v>3400</v>
+        <v>2930</v>
       </c>
       <c r="AC38">
         <f t="shared" si="24"/>
-        <v>3560</v>
+        <v>3090</v>
       </c>
       <c r="AD38">
         <f t="shared" si="16"/>
-        <v>10440</v>
+        <v>9030</v>
       </c>
       <c r="AE38">
         <f t="shared" si="17"/>
-        <v>13700</v>
+        <v>12300</v>
       </c>
       <c r="AF38" s="4">
         <f>AD38+AD39</f>
-        <v>19140</v>
+        <v>16290</v>
       </c>
       <c r="AG38" s="4">
         <f>AE38+AE39</f>
-        <v>23930</v>
+        <v>21150</v>
       </c>
       <c r="AH38" s="4">
         <f t="shared" si="28"/>
-        <v>52990</v>
+        <v>46815</v>
       </c>
       <c r="AI38" s="4">
         <f t="shared" si="29"/>
-        <v>59990</v>
+        <v>54420</v>
       </c>
       <c r="AJ38" s="4">
         <f t="shared" ref="AJ38:AJ42" si="30">AH38-AI38</f>
-        <v>-7000</v>
-      </c>
-      <c r="AK38" s="4"/>
+        <v>-7605</v>
+      </c>
+      <c r="AK38" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="AL38" s="4"/>
       <c r="AM38" s="4"/>
     </row>
@@ -4822,7 +4981,7 @@
       </c>
       <c r="C39">
         <f t="shared" si="25"/>
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>161</v>
@@ -4835,7 +4994,7 @@
       </c>
       <c r="G39" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SCIENTIFIC_THEORY" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SCIENTIFIC_THEORY" /&gt;&lt;Set Cost="960"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H39">
         <f t="shared" si="26"/>
@@ -4849,7 +5008,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="27"/>
-        <v>2820</v>
+        <v>2500</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>164</v>
@@ -4862,7 +5021,7 @@
       </c>
       <c r="O39" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NUCLEAR_PROGRAM" /&gt;&lt;Set Cost="2820"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NUCLEAR_PROGRAM" /&gt;&lt;Set Cost="2500"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P39">
         <v>13</v>
@@ -4889,41 +5048,43 @@
         <v>2</v>
       </c>
       <c r="X39">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="Y39">
         <f t="shared" si="19"/>
-        <v>870</v>
+        <v>620</v>
       </c>
       <c r="Z39">
         <f t="shared" si="20"/>
-        <v>4350</v>
+        <v>3630</v>
       </c>
       <c r="AA39">
         <v>0</v>
       </c>
       <c r="AB39">
         <f t="shared" si="23"/>
-        <v>4350</v>
+        <v>3630</v>
       </c>
       <c r="AC39">
         <f t="shared" si="24"/>
-        <v>4350</v>
+        <v>3630</v>
       </c>
       <c r="AD39">
         <f t="shared" si="16"/>
-        <v>8700</v>
+        <v>7260</v>
       </c>
       <c r="AE39">
         <f t="shared" si="17"/>
-        <v>10230</v>
+        <v>8850</v>
       </c>
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
       <c r="AH39" s="4"/>
       <c r="AI39" s="4"/>
       <c r="AJ39" s="4"/>
-      <c r="AK39" s="4"/>
+      <c r="AK39" s="7" t="s">
+        <v>174</v>
+      </c>
       <c r="AL39" s="4"/>
       <c r="AM39" s="4"/>
     </row>
@@ -4936,7 +5097,7 @@
       </c>
       <c r="C40">
         <f t="shared" si="25"/>
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>161</v>
@@ -4949,7 +5110,7 @@
       </c>
       <c r="G40" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BALLISTICS" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BALLISTICS" /&gt;&lt;Set Cost="960"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H40">
         <f t="shared" si="26"/>
@@ -4963,7 +5124,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="27"/>
-        <v>2130</v>
+        <v>1860</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>164</v>
@@ -4976,7 +5137,7 @@
       </c>
       <c r="O40" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MASS_MEDIA" /&gt;&lt;Set Cost="2130"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MASS_MEDIA" /&gt;&lt;Set Cost="1860"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P40">
         <v>12</v>
@@ -5003,54 +5164,54 @@
         <v>3</v>
       </c>
       <c r="X40">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="Y40">
         <f t="shared" si="19"/>
-        <v>1020</v>
+        <v>680</v>
       </c>
       <c r="Z40">
         <f t="shared" si="20"/>
-        <v>5370</v>
+        <v>4310</v>
       </c>
       <c r="AA40">
         <v>0</v>
       </c>
       <c r="AB40">
         <f t="shared" si="23"/>
-        <v>5370</v>
+        <v>4310</v>
       </c>
       <c r="AC40">
         <f t="shared" si="24"/>
-        <v>5370</v>
+        <v>4310</v>
       </c>
       <c r="AD40">
         <f t="shared" si="16"/>
-        <v>16110</v>
+        <v>12930</v>
       </c>
       <c r="AE40">
         <f t="shared" si="17"/>
-        <v>25200</v>
+        <v>20760</v>
       </c>
       <c r="AF40" s="4">
         <f>AD40+AD41</f>
-        <v>23359</v>
+        <v>18485</v>
       </c>
       <c r="AG40" s="4">
         <f>AE40+AE41</f>
-        <v>40530</v>
+        <v>32730</v>
       </c>
       <c r="AH40" s="4">
         <f t="shared" si="28"/>
-        <v>76349</v>
+        <v>65300</v>
       </c>
       <c r="AI40" s="4">
         <f t="shared" si="29"/>
-        <v>100520</v>
+        <v>87150</v>
       </c>
       <c r="AJ40" s="4">
         <f t="shared" si="30"/>
-        <v>-24171</v>
+        <v>-21850</v>
       </c>
       <c r="AK40" s="5" t="s">
         <v>166</v>
@@ -5067,7 +5228,7 @@
       </c>
       <c r="C41">
         <f t="shared" si="25"/>
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>161</v>
@@ -5080,7 +5241,7 @@
       </c>
       <c r="G41" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_SCIENCE" /&gt;&lt;Set Cost="1000"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_MILITARY_SCIENCE" /&gt;&lt;Set Cost="960"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H41">
         <f t="shared" si="26"/>
@@ -5094,7 +5255,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="27"/>
-        <v>2130</v>
+        <v>1860</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>164</v>
@@ -5107,7 +5268,7 @@
       </c>
       <c r="O41" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MOBILIZATION" /&gt;&lt;Set Cost="2130"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_MOBILIZATION" /&gt;&lt;Set Cost="1860"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P41">
         <v>12</v>
@@ -5133,34 +5294,34 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X41">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="Y41">
         <f t="shared" si="19"/>
-        <v>1220</v>
+        <v>740</v>
       </c>
       <c r="Z41">
         <f t="shared" si="20"/>
-        <v>6590</v>
+        <v>5050</v>
       </c>
       <c r="AA41">
         <v>0</v>
       </c>
       <c r="AB41">
         <f t="shared" si="23"/>
-        <v>6590</v>
+        <v>5050</v>
       </c>
       <c r="AC41">
         <f t="shared" si="24"/>
-        <v>6590</v>
+        <v>5050</v>
       </c>
       <c r="AD41">
         <f t="shared" si="16"/>
-        <v>7249.0000000000009</v>
+        <v>5555</v>
       </c>
       <c r="AE41">
         <f t="shared" si="17"/>
-        <v>15330</v>
+        <v>11970</v>
       </c>
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
@@ -5180,7 +5341,7 @@
       </c>
       <c r="C42">
         <f t="shared" si="25"/>
-        <v>1310</v>
+        <v>1240</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>161</v>
@@ -5193,7 +5354,7 @@
       </c>
       <c r="G42" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEAM_POWER" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEAM_POWER" /&gt;&lt;Set Cost="1240"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H42">
         <f t="shared" si="26"/>
@@ -5207,7 +5368,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="27"/>
-        <v>2700</v>
+        <v>2380</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>164</v>
@@ -5220,7 +5381,7 @@
       </c>
       <c r="O42" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_IDEOLOGY" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_IDEOLOGY" /&gt;&lt;Set Cost="2380"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P42">
         <v>13</v>
@@ -5246,58 +5407,58 @@
         <v>1</v>
       </c>
       <c r="X42">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="Y42">
         <f t="shared" si="19"/>
-        <v>1420</v>
+        <v>800</v>
       </c>
       <c r="Z42">
         <f t="shared" si="20"/>
-        <v>8010</v>
+        <v>5850</v>
       </c>
       <c r="AA42">
         <v>0</v>
       </c>
       <c r="AB42">
         <f t="shared" si="23"/>
-        <v>8010</v>
+        <v>5850</v>
       </c>
       <c r="AC42">
         <f t="shared" si="24"/>
-        <v>8010</v>
+        <v>5850</v>
       </c>
       <c r="AD42">
         <f t="shared" si="16"/>
-        <v>8010</v>
+        <v>5850</v>
       </c>
       <c r="AE42">
         <f t="shared" si="17"/>
-        <v>36960</v>
+        <v>27240</v>
       </c>
       <c r="AF42" s="4">
         <f>AD42+AD43</f>
-        <v>46530</v>
+        <v>32690</v>
       </c>
       <c r="AG42" s="4">
         <f>AE42+AE43</f>
-        <v>44310</v>
+        <v>32350</v>
       </c>
       <c r="AH42" s="4">
         <f t="shared" ref="AH42:AI42" si="31">AH40+AF42</f>
-        <v>122879</v>
+        <v>97990</v>
       </c>
       <c r="AI42" s="4">
         <f t="shared" si="31"/>
-        <v>144830</v>
+        <v>119500</v>
       </c>
       <c r="AJ42" s="4">
         <f t="shared" si="30"/>
-        <v>-21951</v>
+        <v>-21510</v>
       </c>
       <c r="AK42" s="4">
         <f>Z43+0.5*Y44</f>
-        <v>10065</v>
+        <v>6955</v>
       </c>
       <c r="AL42" s="4"/>
       <c r="AM42" s="4"/>
@@ -5311,7 +5472,7 @@
       </c>
       <c r="C43">
         <f t="shared" si="25"/>
-        <v>1310</v>
+        <v>1240</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>161</v>
@@ -5324,7 +5485,7 @@
       </c>
       <c r="G43" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SANITATION" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SANITATION" /&gt;&lt;Set Cost="1240"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H43">
         <f t="shared" si="26"/>
@@ -5338,7 +5499,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="27"/>
-        <v>2700</v>
+        <v>2380</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>164</v>
@@ -5351,7 +5512,7 @@
       </c>
       <c r="O43" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SUFFRAGE" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SUFFRAGE" /&gt;&lt;Set Cost="2380"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P43">
         <v>13</v>
@@ -5378,34 +5539,34 @@
         <v>4</v>
       </c>
       <c r="X43">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="Y43">
         <f t="shared" si="19"/>
-        <v>1620</v>
+        <v>860</v>
       </c>
       <c r="Z43">
         <f t="shared" si="20"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="AA43">
         <v>0</v>
       </c>
       <c r="AB43">
         <f t="shared" si="23"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="AC43">
         <f t="shared" si="24"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="AD43">
         <f t="shared" si="16"/>
-        <v>38520</v>
+        <v>26840</v>
       </c>
       <c r="AE43">
         <f t="shared" si="17"/>
-        <v>7350</v>
+        <v>5110</v>
       </c>
       <c r="AF43" s="4"/>
       <c r="AG43" s="4"/>
@@ -5425,7 +5586,7 @@
       </c>
       <c r="C44">
         <f t="shared" si="25"/>
-        <v>1310</v>
+        <v>1240</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>161</v>
@@ -5438,7 +5599,7 @@
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ECONOMICS" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ECONOMICS" /&gt;&lt;Set Cost="1240"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H44">
         <f t="shared" si="26"/>
@@ -5452,7 +5613,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="27"/>
-        <v>2700</v>
+        <v>2380</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>164</v>
@@ -5465,7 +5626,7 @@
       </c>
       <c r="O44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_TOTALITARIANISM" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_TOTALITARIANISM" /&gt;&lt;Set Cost="2380"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P44">
         <v>13</v>
@@ -5491,54 +5652,54 @@
         <v>1</v>
       </c>
       <c r="X44">
-        <v>-750</v>
+        <v>-370</v>
       </c>
       <c r="Y44">
         <f>Y43+X44</f>
-        <v>870</v>
+        <v>490</v>
       </c>
       <c r="Z44">
         <f>Z43+Y44</f>
-        <v>10500</v>
+        <v>7200</v>
       </c>
       <c r="AA44">
         <v>0</v>
       </c>
       <c r="AB44">
         <f t="shared" si="23"/>
-        <v>10500</v>
+        <v>7200</v>
       </c>
       <c r="AC44">
         <f t="shared" si="24"/>
-        <v>10500</v>
+        <v>7200</v>
       </c>
       <c r="AD44">
         <f t="shared" si="16"/>
-        <v>10500</v>
+        <v>7200</v>
       </c>
       <c r="AE44">
         <f t="shared" si="17"/>
-        <v>8000</v>
+        <v>5400</v>
       </c>
       <c r="AF44" s="2">
         <f>AD44</f>
-        <v>10500</v>
+        <v>7200</v>
       </c>
       <c r="AG44" s="2">
         <f>AE44</f>
-        <v>8000</v>
+        <v>5400</v>
       </c>
       <c r="AH44">
         <f t="shared" ref="AH44:AI44" si="32">AH42+AF44</f>
-        <v>133379</v>
+        <v>105190</v>
       </c>
       <c r="AI44">
         <f t="shared" si="32"/>
-        <v>152830</v>
+        <v>124900</v>
       </c>
       <c r="AJ44">
         <f>AH44-AI44</f>
-        <v>-19451</v>
+        <v>-19710</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
@@ -5550,7 +5711,7 @@
       </c>
       <c r="C45">
         <f t="shared" si="25"/>
-        <v>1310</v>
+        <v>1240</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>161</v>
@@ -5563,7 +5724,7 @@
       </c>
       <c r="G45" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RIFLING" /&gt;&lt;Set Cost="1310"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RIFLING" /&gt;&lt;Set Cost="1240"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H45">
         <f t="shared" si="26"/>
@@ -5577,7 +5738,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="27"/>
-        <v>2700</v>
+        <v>2380</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>164</v>
@@ -5590,7 +5751,7 @@
       </c>
       <c r="O45" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CLASS_STRUGGLE" /&gt;&lt;Set Cost="2700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CLASS_STRUGGLE" /&gt;&lt;Set Cost="2380"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P45">
         <v>13</v>
@@ -5605,7 +5766,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="25"/>
-        <v>1700</v>
+        <v>1540</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>161</v>
@@ -5618,7 +5779,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FLIGHT" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FLIGHT" /&gt;&lt;Set Cost="1540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H46">
         <f t="shared" si="26"/>
@@ -5632,7 +5793,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="27"/>
-        <v>3560</v>
+        <v>3090</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>164</v>
@@ -5645,7 +5806,7 @@
       </c>
       <c r="O46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLD_WAR" /&gt;&lt;Set Cost="3560"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_COLD_WAR" /&gt;&lt;Set Cost="3090"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P46">
         <v>14</v>
@@ -5655,7 +5816,7 @@
       </c>
       <c r="T46">
         <f>AB25</f>
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
@@ -5667,7 +5828,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="25"/>
-        <v>1700</v>
+        <v>1540</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>161</v>
@@ -5680,7 +5841,7 @@
       </c>
       <c r="G47" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REPLACEABLE_PARTS" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REPLACEABLE_PARTS" /&gt;&lt;Set Cost="1540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H47">
         <f t="shared" si="26"/>
@@ -5694,7 +5855,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="27"/>
-        <v>3560</v>
+        <v>3090</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>164</v>
@@ -5707,7 +5868,7 @@
       </c>
       <c r="O47" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_PROFESSIONAL_SPORTS" /&gt;&lt;Set Cost="3560"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_PROFESSIONAL_SPORTS" /&gt;&lt;Set Cost="3090"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P47">
         <v>14</v>
@@ -5717,7 +5878,7 @@
       </c>
       <c r="T47">
         <f>AB26</f>
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
@@ -5729,7 +5890,7 @@
       </c>
       <c r="C48">
         <f t="shared" si="25"/>
-        <v>1700</v>
+        <v>1540</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>161</v>
@@ -5742,7 +5903,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEEL" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEEL" /&gt;&lt;Set Cost="1540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H48">
         <f t="shared" si="26"/>
@@ -5756,7 +5917,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="27"/>
-        <v>3400</v>
+        <v>2930</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>164</v>
@@ -5769,7 +5930,7 @@
       </c>
       <c r="O48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HERITAGE" /&gt;&lt;Set Cost="3400"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HERITAGE" /&gt;&lt;Set Cost="2930"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P48">
         <v>14</v>
@@ -5779,7 +5940,7 @@
       </c>
       <c r="T48">
         <f>AB27</f>
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
@@ -5791,7 +5952,7 @@
       </c>
       <c r="C49">
         <f t="shared" si="25"/>
-        <v>2170</v>
+        <v>1990</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>161</v>
@@ -5804,7 +5965,7 @@
       </c>
       <c r="G49" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ELECTRICITY" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ELECTRICITY" /&gt;&lt;Set Cost="1990"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H49">
         <f t="shared" si="26"/>
@@ -5818,7 +5979,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="27"/>
-        <v>4350</v>
+        <v>3630</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>164</v>
@@ -5831,7 +5992,7 @@
       </c>
       <c r="O49" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RAPID_DEPLOYMENT" /&gt;&lt;Set Cost="4350"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_RAPID_DEPLOYMENT" /&gt;&lt;Set Cost="3630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P49">
         <v>15</v>
@@ -5841,7 +6002,7 @@
       </c>
       <c r="T49">
         <f>AC27</f>
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
@@ -5853,7 +6014,7 @@
       </c>
       <c r="C50">
         <f t="shared" si="25"/>
-        <v>2170</v>
+        <v>1990</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>161</v>
@@ -5866,7 +6027,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RADIO" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_RADIO" /&gt;&lt;Set Cost="1990"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H50">
         <f t="shared" si="26"/>
@@ -5880,7 +6041,7 @@
       </c>
       <c r="K50">
         <f t="shared" si="27"/>
-        <v>4350</v>
+        <v>3630</v>
       </c>
       <c r="L50" s="3" t="s">
         <v>164</v>
@@ -5893,7 +6054,7 @@
       </c>
       <c r="O50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SPACE_RACE" /&gt;&lt;Set Cost="4350"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SPACE_RACE" /&gt;&lt;Set Cost="3630"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P50">
         <v>15</v>
@@ -5903,7 +6064,7 @@
       </c>
       <c r="T50">
         <f>AB28</f>
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
@@ -5915,7 +6076,7 @@
       </c>
       <c r="C51">
         <f t="shared" si="25"/>
-        <v>2170</v>
+        <v>1990</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>161</v>
@@ -5928,7 +6089,7 @@
       </c>
       <c r="G51" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CHEMISTRY" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CHEMISTRY" /&gt;&lt;Set Cost="1990"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H51">
         <f t="shared" si="26"/>
@@ -5942,7 +6103,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="27"/>
-        <v>5370</v>
+        <v>4310</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>164</v>
@@ -5955,7 +6116,7 @@
       </c>
       <c r="O51" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBALIZATION" /&gt;&lt;Set Cost="5370"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBALIZATION" /&gt;&lt;Set Cost="4310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P51">
         <v>16</v>
@@ -5965,7 +6126,7 @@
       </c>
       <c r="T51">
         <f>AB29</f>
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
@@ -5977,7 +6138,7 @@
       </c>
       <c r="C52">
         <f t="shared" si="25"/>
-        <v>2170</v>
+        <v>1990</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>161</v>
@@ -5990,7 +6151,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBUSTION" /&gt;&lt;Set Cost="2170"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBUSTION" /&gt;&lt;Set Cost="1990"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H52">
         <f t="shared" si="26"/>
@@ -6004,7 +6165,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="27"/>
-        <v>5370</v>
+        <v>4310</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>164</v>
@@ -6017,7 +6178,7 @@
       </c>
       <c r="O52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SOCIAL_MEDIA" /&gt;&lt;Set Cost="5370"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SOCIAL_MEDIA" /&gt;&lt;Set Cost="4310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P52">
         <v>16</v>
@@ -6027,7 +6188,7 @@
       </c>
       <c r="T52">
         <f>AC29</f>
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -6039,7 +6200,7 @@
       </c>
       <c r="C53">
         <f t="shared" si="25"/>
-        <v>2740</v>
+        <v>2460</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>161</v>
@@ -6052,7 +6213,7 @@
       </c>
       <c r="G53" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_FLIGHT" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_FLIGHT" /&gt;&lt;Set Cost="2460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H53">
         <f t="shared" si="26"/>
@@ -6066,7 +6227,7 @@
       </c>
       <c r="K53">
         <f t="shared" si="27"/>
-        <v>10500</v>
+        <v>7200</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>164</v>
@@ -6079,7 +6240,7 @@
       </c>
       <c r="O53" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FUTURE_CIVIC" /&gt;&lt;Set Cost="10500"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_FUTURE_CIVIC" /&gt;&lt;Set Cost="7200"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P53">
         <v>20</v>
@@ -6089,7 +6250,7 @@
       </c>
       <c r="T53">
         <f>AB30</f>
-        <v>355</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
@@ -6101,7 +6262,7 @@
       </c>
       <c r="C54">
         <f t="shared" si="25"/>
-        <v>2740</v>
+        <v>2460</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>161</v>
@@ -6114,7 +6275,7 @@
       </c>
       <c r="G54" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROCKETRY" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROCKETRY" /&gt;&lt;Set Cost="2460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H54">
         <f t="shared" si="26"/>
@@ -6128,7 +6289,7 @@
       </c>
       <c r="K54">
         <f t="shared" si="27"/>
-        <v>5370</v>
+        <v>4310</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>164</v>
@@ -6141,7 +6302,7 @@
       </c>
       <c r="O54" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_ENVIRONMENTALISM" /&gt;&lt;Set Cost="5370"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_ENVIRONMENTALISM" /&gt;&lt;Set Cost="4310"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P54">
         <v>16</v>
@@ -6151,7 +6312,7 @@
       </c>
       <c r="T54">
         <f>AC30</f>
-        <v>445</v>
+        <v>425</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
@@ -6163,7 +6324,7 @@
       </c>
       <c r="C55">
         <f t="shared" si="25"/>
-        <v>2740</v>
+        <v>2460</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>161</v>
@@ -6176,7 +6337,7 @@
       </c>
       <c r="G55" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_BALLISTICS" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_BALLISTICS" /&gt;&lt;Set Cost="2460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H55">
         <f t="shared" si="26"/>
@@ -6190,7 +6351,7 @@
       </c>
       <c r="K55">
         <f t="shared" si="27"/>
-        <v>6590</v>
+        <v>5050</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>164</v>
@@ -6203,7 +6364,7 @@
       </c>
       <c r="O55" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CORPORATE_LIBERTARIANISM" /&gt;&lt;Set Cost="6590"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CORPORATE_LIBERTARIANISM" /&gt;&lt;Set Cost="5050"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P55">
         <v>17</v>
@@ -6213,7 +6374,7 @@
       </c>
       <c r="T55">
         <f>AB31</f>
-        <v>505</v>
+        <v>465</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
@@ -6225,7 +6386,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="25"/>
-        <v>2740</v>
+        <v>2460</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>161</v>
@@ -6238,7 +6399,7 @@
       </c>
       <c r="G56" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBINED_ARMS" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMBINED_ARMS" /&gt;&lt;Set Cost="2460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H56">
         <f t="shared" si="26"/>
@@ -6252,7 +6413,7 @@
       </c>
       <c r="K56">
         <f t="shared" si="27"/>
-        <v>6590</v>
+        <v>5050</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>164</v>
@@ -6265,7 +6426,7 @@
       </c>
       <c r="O56" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIGITAL_DEMOCRACY" /&gt;&lt;Set Cost="6590"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_DIGITAL_DEMOCRACY" /&gt;&lt;Set Cost="5050"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P56">
         <v>17</v>
@@ -6275,7 +6436,7 @@
       </c>
       <c r="T56">
         <f>AC31</f>
-        <v>595</v>
+        <v>555</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
@@ -6287,7 +6448,7 @@
       </c>
       <c r="C57">
         <f t="shared" si="25"/>
-        <v>2740</v>
+        <v>2460</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>161</v>
@@ -6300,7 +6461,7 @@
       </c>
       <c r="G57" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PLASTICS" /&gt;&lt;Set Cost="2740"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PLASTICS" /&gt;&lt;Set Cost="2460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H57">
         <f t="shared" si="26"/>
@@ -6314,7 +6475,7 @@
       </c>
       <c r="K57">
         <f t="shared" si="27"/>
-        <v>6590</v>
+        <v>5050</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>164</v>
@@ -6327,7 +6488,7 @@
       </c>
       <c r="O57" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SYNTHETIC_TECHNOCRACY" /&gt;&lt;Set Cost="6590"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SYNTHETIC_TECHNOCRACY" /&gt;&lt;Set Cost="5050"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P57">
         <v>17</v>
@@ -6337,7 +6498,7 @@
       </c>
       <c r="T57">
         <f>AB32</f>
-        <v>690</v>
+        <v>630</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
@@ -6349,7 +6510,7 @@
       </c>
       <c r="C58">
         <f t="shared" si="25"/>
-        <v>3410</v>
+        <v>2950</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>161</v>
@@ -6362,7 +6523,7 @@
       </c>
       <c r="G58" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPUTERS" /&gt;&lt;Set Cost="3410"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPUTERS" /&gt;&lt;Set Cost="2950"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H58">
         <f t="shared" si="26"/>
@@ -6376,7 +6537,7 @@
       </c>
       <c r="K58">
         <f t="shared" si="27"/>
-        <v>8010</v>
+        <v>5850</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>164</v>
@@ -6389,7 +6550,7 @@
       </c>
       <c r="O58" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NEAR_FUTURE_GOVERNANCE" /&gt;&lt;Set Cost="8010"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_NEAR_FUTURE_GOVERNANCE" /&gt;&lt;Set Cost="5850"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P58">
         <v>17</v>
@@ -6399,7 +6560,7 @@
       </c>
       <c r="T58">
         <f>AC32</f>
-        <v>810</v>
+        <v>750</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
@@ -6411,7 +6572,7 @@
       </c>
       <c r="C59">
         <f t="shared" si="25"/>
-        <v>3410</v>
+        <v>2950</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>161</v>
@@ -6424,7 +6585,7 @@
       </c>
       <c r="G59" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FISSION" /&gt;&lt;Set Cost="3410"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FISSION" /&gt;&lt;Set Cost="2950"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H59">
         <f t="shared" si="26"/>
@@ -6438,7 +6599,7 @@
       </c>
       <c r="K59">
         <f t="shared" si="27"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>164</v>
@@ -6451,7 +6612,7 @@
       </c>
       <c r="O59" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBAL_WARMING_MITIGATION" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_GLOBAL_WARMING_MITIGATION" /&gt;&lt;Set Cost="6710"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P59">
         <v>18</v>
@@ -6461,7 +6622,7 @@
       </c>
       <c r="T59">
         <f>AB33</f>
-        <v>1000</v>
+        <v>900</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
@@ -6473,7 +6634,7 @@
       </c>
       <c r="C60">
         <f t="shared" si="25"/>
-        <v>3410</v>
+        <v>2950</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>161</v>
@@ -6486,7 +6647,7 @@
       </c>
       <c r="G60" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SYNTHETIC_MATERIALS" /&gt;&lt;Set Cost="3410"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SYNTHETIC_MATERIALS" /&gt;&lt;Set Cost="2950"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H60">
         <f t="shared" si="26"/>
@@ -6500,7 +6661,7 @@
       </c>
       <c r="K60">
         <f t="shared" si="27"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>164</v>
@@ -6513,7 +6674,7 @@
       </c>
       <c r="O60" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SMART_POWER_DOCTRINE" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_SMART_POWER_DOCTRINE" /&gt;&lt;Set Cost="6710"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P60">
         <v>19</v>
@@ -6523,7 +6684,7 @@
       </c>
       <c r="T60">
         <f>AB34</f>
-        <v>1245</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
@@ -6535,7 +6696,7 @@
       </c>
       <c r="C61">
         <f t="shared" si="25"/>
-        <v>4200</v>
+        <v>3460</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>161</v>
@@ -6548,7 +6709,7 @@
       </c>
       <c r="G61" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_TELECOMMUNICATIONS" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_TELECOMMUNICATIONS" /&gt;&lt;Set Cost="3460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H61">
         <f t="shared" si="26"/>
@@ -6562,7 +6723,7 @@
       </c>
       <c r="K61">
         <f t="shared" si="27"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>164</v>
@@ -6575,7 +6736,7 @@
       </c>
       <c r="O61" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_INFORMATION_WARFARE" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_INFORMATION_WARFARE" /&gt;&lt;Set Cost="6710"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P61">
         <v>19</v>
@@ -6585,7 +6746,7 @@
       </c>
       <c r="T61">
         <f>AC34</f>
-        <v>1395</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
@@ -6597,7 +6758,7 @@
       </c>
       <c r="C62">
         <f t="shared" si="25"/>
-        <v>4200</v>
+        <v>3460</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>161</v>
@@ -6610,7 +6771,7 @@
       </c>
       <c r="G62" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SATELLITES" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SATELLITES" /&gt;&lt;Set Cost="3460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H62">
         <f t="shared" si="26"/>
@@ -6624,7 +6785,7 @@
       </c>
       <c r="K62">
         <f t="shared" si="27"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>164</v>
@@ -6637,7 +6798,7 @@
       </c>
       <c r="O62" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXODUS_IMPERATIVE" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_EXODUS_IMPERATIVE" /&gt;&lt;Set Cost="6710"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P62">
         <v>19</v>
@@ -6647,7 +6808,7 @@
       </c>
       <c r="T62">
         <f>AB35</f>
-        <v>1635</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
@@ -6659,7 +6820,7 @@
       </c>
       <c r="C63">
         <f t="shared" si="25"/>
-        <v>4200</v>
+        <v>3460</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>161</v>
@@ -6672,7 +6833,7 @@
       </c>
       <c r="G63" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUIDANCE_SYSTEMS" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_GUIDANCE_SYSTEMS" /&gt;&lt;Set Cost="3460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H63">
         <f t="shared" si="26"/>
@@ -6686,7 +6847,7 @@
       </c>
       <c r="K63">
         <f t="shared" si="27"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
       <c r="L63" s="3" t="s">
         <v>164</v>
@@ -6699,7 +6860,7 @@
       </c>
       <c r="O63" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HEGEMONY" /&gt;&lt;Set Cost="9630"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where CivicType="CIVIC_CULTURAL_HEGEMONY" /&gt;&lt;Set Cost="6710"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="P63">
         <v>19</v>
@@ -6709,7 +6870,7 @@
       </c>
       <c r="T63">
         <f>AC35</f>
-        <v>1785</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
@@ -6721,7 +6882,7 @@
       </c>
       <c r="C64">
         <f t="shared" si="25"/>
-        <v>4200</v>
+        <v>3460</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>161</v>
@@ -6734,7 +6895,7 @@
       </c>
       <c r="G64" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_LASERS" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_LASERS" /&gt;&lt;Set Cost="3460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H64">
         <f t="shared" si="26"/>
@@ -6749,7 +6910,7 @@
       </c>
       <c r="T64">
         <f>AB36</f>
-        <v>2130</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
@@ -6761,7 +6922,7 @@
       </c>
       <c r="C65">
         <f t="shared" si="25"/>
-        <v>4200</v>
+        <v>3460</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>161</v>
@@ -6774,7 +6935,7 @@
       </c>
       <c r="G65" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPOSITES" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_COMPOSITES" /&gt;&lt;Set Cost="3460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H65">
         <f t="shared" si="26"/>
@@ -6789,7 +6950,7 @@
       </c>
       <c r="T65">
         <f>AC36</f>
-        <v>2250</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
@@ -6801,7 +6962,7 @@
       </c>
       <c r="C66">
         <f t="shared" si="25"/>
-        <v>4200</v>
+        <v>3460</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>161</v>
@@ -6814,7 +6975,7 @@
       </c>
       <c r="G66" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEALTH_TECHNOLOGY" /&gt;&lt;Set Cost="4200"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_STEALTH_TECHNOLOGY" /&gt;&lt;Set Cost="3460"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H66">
         <f t="shared" si="26"/>
@@ -6829,7 +6990,7 @@
       </c>
       <c r="T66">
         <f>AB37</f>
-        <v>2700</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
@@ -6841,7 +7002,7 @@
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C79" si="33">VLOOKUP(B67,$T$3:$AB$22,9,FALSE)</f>
-        <v>5110</v>
+        <v>3990</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>161</v>
@@ -6854,7 +7015,7 @@
       </c>
       <c r="G67" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROBOTICS" /&gt;&lt;Set Cost="5110"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ROBOTICS" /&gt;&lt;Set Cost="3990"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H79" si="34">VLOOKUP(B67,$T$3:$U$22,2,FALSE)</f>
@@ -6869,7 +7030,7 @@
       </c>
       <c r="T67">
         <f>AC37</f>
-        <v>2820</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
@@ -6881,7 +7042,7 @@
       </c>
       <c r="C68">
         <f t="shared" si="33"/>
-        <v>5110</v>
+        <v>3990</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>161</v>
@@ -6894,7 +7055,7 @@
       </c>
       <c r="G68" s="3" t="str">
         <f t="shared" ref="G68:G79" si="35">_xlfn.CONCAT(D68,A68,E68,C68,F68)</f>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NANOTECHNOLOGY" /&gt;&lt;Set Cost="5110"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NANOTECHNOLOGY" /&gt;&lt;Set Cost="3990"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H68">
         <f t="shared" si="34"/>
@@ -6909,7 +7070,7 @@
       </c>
       <c r="T68">
         <f>AB38</f>
-        <v>3400</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
@@ -6921,7 +7082,7 @@
       </c>
       <c r="C69">
         <f t="shared" si="33"/>
-        <v>5110</v>
+        <v>3990</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>161</v>
@@ -6934,7 +7095,7 @@
       </c>
       <c r="G69" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FUSION" /&gt;&lt;Set Cost="5110"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_NUCLEAR_FUSION" /&gt;&lt;Set Cost="3990"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H69">
         <f t="shared" si="34"/>
@@ -6949,7 +7110,7 @@
       </c>
       <c r="T69">
         <f>AC38</f>
-        <v>3560</v>
+        <v>3090</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
@@ -6961,7 +7122,7 @@
       </c>
       <c r="C70">
         <f t="shared" si="33"/>
-        <v>320</v>
+        <v>280</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>161</v>
@@ -6974,7 +7135,7 @@
       </c>
       <c r="G70" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BUTTRESS" /&gt;&lt;Set Cost="320"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_BUTTRESS" /&gt;&lt;Set Cost="280"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H70">
         <f t="shared" si="34"/>
@@ -6989,7 +7150,7 @@
       </c>
       <c r="T70">
         <f t="shared" ref="T70:T75" si="36">AB39</f>
-        <v>4350</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
@@ -7001,7 +7162,7 @@
       </c>
       <c r="C71">
         <f t="shared" si="33"/>
-        <v>1700</v>
+        <v>1540</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>161</v>
@@ -7014,7 +7175,7 @@
       </c>
       <c r="G71" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REFINING" /&gt;&lt;Set Cost="1700"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_REFINING" /&gt;&lt;Set Cost="1540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H71">
         <f t="shared" si="34"/>
@@ -7029,7 +7190,7 @@
       </c>
       <c r="T71">
         <f t="shared" si="36"/>
-        <v>5370</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
@@ -7041,7 +7202,7 @@
       </c>
       <c r="C72">
         <f t="shared" si="33"/>
-        <v>6160</v>
+        <v>4540</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>161</v>
@@ -7054,7 +7215,7 @@
       </c>
       <c r="G72" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SEASTEADS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SEASTEADS" /&gt;&lt;Set Cost="4540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H72">
         <f t="shared" si="34"/>
@@ -7069,7 +7230,7 @@
       </c>
       <c r="T72">
         <f t="shared" si="36"/>
-        <v>6590</v>
+        <v>5050</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
@@ -7081,7 +7242,7 @@
       </c>
       <c r="C73">
         <f t="shared" si="33"/>
-        <v>6160</v>
+        <v>4540</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>161</v>
@@ -7094,7 +7255,7 @@
       </c>
       <c r="G73" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_AI" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_AI" /&gt;&lt;Set Cost="4540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H73">
         <f t="shared" si="34"/>
@@ -7109,7 +7270,7 @@
       </c>
       <c r="T73">
         <f t="shared" si="36"/>
-        <v>8010</v>
+        <v>5850</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
@@ -7121,7 +7282,7 @@
       </c>
       <c r="C74">
         <f t="shared" si="33"/>
-        <v>6160</v>
+        <v>4540</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>161</v>
@@ -7134,7 +7295,7 @@
       </c>
       <c r="G74" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_POWER_CELLS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_ADVANCED_POWER_CELLS" /&gt;&lt;Set Cost="4540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H74">
         <f t="shared" si="34"/>
@@ -7149,7 +7310,7 @@
       </c>
       <c r="T74">
         <f t="shared" si="36"/>
-        <v>9630</v>
+        <v>6710</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
@@ -7161,7 +7322,7 @@
       </c>
       <c r="C75">
         <f t="shared" si="33"/>
-        <v>6160</v>
+        <v>4540</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>161</v>
@@ -7174,7 +7335,7 @@
       </c>
       <c r="G75" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CYBERNETICS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_CYBERNETICS" /&gt;&lt;Set Cost="4540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H75">
         <f t="shared" si="34"/>
@@ -7189,7 +7350,7 @@
       </c>
       <c r="T75">
         <f t="shared" si="36"/>
-        <v>10500</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
@@ -7201,7 +7362,7 @@
       </c>
       <c r="C76">
         <f t="shared" si="33"/>
-        <v>6160</v>
+        <v>4540</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>161</v>
@@ -7214,7 +7375,7 @@
       </c>
       <c r="G76" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SMART_MATERIALS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_SMART_MATERIALS" /&gt;&lt;Set Cost="4540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H76">
         <f t="shared" si="34"/>
@@ -7234,7 +7395,7 @@
       </c>
       <c r="C77">
         <f t="shared" si="33"/>
-        <v>6160</v>
+        <v>4540</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>161</v>
@@ -7247,7 +7408,7 @@
       </c>
       <c r="G77" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PREDICTIVE_SYSTEMS" /&gt;&lt;Set Cost="6160"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_PREDICTIVE_SYSTEMS" /&gt;&lt;Set Cost="4540"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H77">
         <f t="shared" si="34"/>
@@ -7267,7 +7428,7 @@
       </c>
       <c r="C78">
         <f t="shared" si="33"/>
-        <v>7350</v>
+        <v>5110</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>161</v>
@@ -7280,7 +7441,7 @@
       </c>
       <c r="G78" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_OFFWORLD_MISSION" /&gt;&lt;Set Cost="7350"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_OFFWORLD_MISSION" /&gt;&lt;Set Cost="5110"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H78">
         <f t="shared" si="34"/>
@@ -7300,7 +7461,7 @@
       </c>
       <c r="C79">
         <f t="shared" si="33"/>
-        <v>8000</v>
+        <v>5400</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>161</v>
@@ -7313,7 +7474,7 @@
       </c>
       <c r="G79" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FUTURE_TECH" /&gt;&lt;Set Cost="8000"/&gt;&lt;/Update&gt;</v>
+        <v>&lt;Update&gt;&lt;Where TechnologyType="TECH_FUTURE_TECH" /&gt;&lt;Set Cost="5400"/&gt;&lt;/Update&gt;</v>
       </c>
       <c r="H79">
         <f t="shared" si="34"/>
@@ -7325,7 +7486,56 @@
       <c r="O79" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="65">
+    <mergeCell ref="AL42:AL43"/>
+    <mergeCell ref="AM25:AM27"/>
+    <mergeCell ref="AM28:AM29"/>
+    <mergeCell ref="AM30:AM31"/>
+    <mergeCell ref="AM32:AM33"/>
+    <mergeCell ref="AM34:AM35"/>
+    <mergeCell ref="AM36:AM37"/>
+    <mergeCell ref="AM38:AM39"/>
+    <mergeCell ref="AM40:AM41"/>
+    <mergeCell ref="AM42:AM43"/>
+    <mergeCell ref="AL25:AL27"/>
+    <mergeCell ref="AL28:AL29"/>
+    <mergeCell ref="AL30:AL31"/>
+    <mergeCell ref="AL32:AL33"/>
+    <mergeCell ref="AL34:AL35"/>
+    <mergeCell ref="AJ38:AJ39"/>
+    <mergeCell ref="AJ40:AJ41"/>
+    <mergeCell ref="AL36:AL37"/>
+    <mergeCell ref="AL38:AL39"/>
+    <mergeCell ref="AL40:AL41"/>
+    <mergeCell ref="AJ42:AJ43"/>
+    <mergeCell ref="AK40:AK41"/>
+    <mergeCell ref="AK42:AK43"/>
+    <mergeCell ref="AJ25:AJ27"/>
+    <mergeCell ref="AJ28:AJ29"/>
+    <mergeCell ref="AJ30:AJ31"/>
+    <mergeCell ref="AJ32:AJ33"/>
+    <mergeCell ref="AJ34:AJ35"/>
+    <mergeCell ref="AJ36:AJ37"/>
+    <mergeCell ref="AH42:AH43"/>
+    <mergeCell ref="AI25:AI27"/>
+    <mergeCell ref="AI28:AI29"/>
+    <mergeCell ref="AI30:AI31"/>
+    <mergeCell ref="AI32:AI33"/>
+    <mergeCell ref="AI34:AI35"/>
+    <mergeCell ref="AI36:AI37"/>
+    <mergeCell ref="AI38:AI39"/>
+    <mergeCell ref="AI40:AI41"/>
+    <mergeCell ref="AI42:AI43"/>
+    <mergeCell ref="AH25:AH27"/>
+    <mergeCell ref="AH28:AH29"/>
+    <mergeCell ref="AH30:AH31"/>
+    <mergeCell ref="AH32:AH33"/>
+    <mergeCell ref="AH34:AH35"/>
+    <mergeCell ref="AF38:AF39"/>
+    <mergeCell ref="AF40:AF41"/>
+    <mergeCell ref="AH36:AH37"/>
+    <mergeCell ref="AH38:AH39"/>
+    <mergeCell ref="AH40:AH41"/>
     <mergeCell ref="AF42:AF43"/>
     <mergeCell ref="AG25:AG27"/>
     <mergeCell ref="AG28:AG29"/>
@@ -7342,62 +7552,6 @@
     <mergeCell ref="AF32:AF33"/>
     <mergeCell ref="AF34:AF35"/>
     <mergeCell ref="AF36:AF37"/>
-    <mergeCell ref="AF38:AF39"/>
-    <mergeCell ref="AF40:AF41"/>
-    <mergeCell ref="AH36:AH37"/>
-    <mergeCell ref="AH38:AH39"/>
-    <mergeCell ref="AH40:AH41"/>
-    <mergeCell ref="AH42:AH43"/>
-    <mergeCell ref="AI25:AI27"/>
-    <mergeCell ref="AI28:AI29"/>
-    <mergeCell ref="AI30:AI31"/>
-    <mergeCell ref="AI32:AI33"/>
-    <mergeCell ref="AI34:AI35"/>
-    <mergeCell ref="AI36:AI37"/>
-    <mergeCell ref="AI38:AI39"/>
-    <mergeCell ref="AI40:AI41"/>
-    <mergeCell ref="AI42:AI43"/>
-    <mergeCell ref="AH25:AH27"/>
-    <mergeCell ref="AH28:AH29"/>
-    <mergeCell ref="AH30:AH31"/>
-    <mergeCell ref="AH32:AH33"/>
-    <mergeCell ref="AH34:AH35"/>
-    <mergeCell ref="AJ42:AJ43"/>
-    <mergeCell ref="AK25:AK27"/>
-    <mergeCell ref="AK28:AK29"/>
-    <mergeCell ref="AK30:AK31"/>
-    <mergeCell ref="AK32:AK33"/>
-    <mergeCell ref="AK34:AK35"/>
-    <mergeCell ref="AK36:AK37"/>
-    <mergeCell ref="AK38:AK39"/>
-    <mergeCell ref="AK40:AK41"/>
-    <mergeCell ref="AK42:AK43"/>
-    <mergeCell ref="AJ25:AJ27"/>
-    <mergeCell ref="AJ28:AJ29"/>
-    <mergeCell ref="AJ30:AJ31"/>
-    <mergeCell ref="AJ32:AJ33"/>
-    <mergeCell ref="AJ34:AJ35"/>
-    <mergeCell ref="AJ36:AJ37"/>
-    <mergeCell ref="AJ38:AJ39"/>
-    <mergeCell ref="AJ40:AJ41"/>
-    <mergeCell ref="AL36:AL37"/>
-    <mergeCell ref="AL38:AL39"/>
-    <mergeCell ref="AL40:AL41"/>
-    <mergeCell ref="AL42:AL43"/>
-    <mergeCell ref="AM25:AM27"/>
-    <mergeCell ref="AM28:AM29"/>
-    <mergeCell ref="AM30:AM31"/>
-    <mergeCell ref="AM32:AM33"/>
-    <mergeCell ref="AM34:AM35"/>
-    <mergeCell ref="AM36:AM37"/>
-    <mergeCell ref="AM38:AM39"/>
-    <mergeCell ref="AM40:AM41"/>
-    <mergeCell ref="AM42:AM43"/>
-    <mergeCell ref="AL25:AL27"/>
-    <mergeCell ref="AL28:AL29"/>
-    <mergeCell ref="AL30:AL31"/>
-    <mergeCell ref="AL32:AL33"/>
-    <mergeCell ref="AL34:AL35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>